<commit_message>
Quite a few updates. BEA GUI signifciantly updated with nearly complete custom Fisher Index creation. Other stuff cleaned up somewhat...t
</commit_message>
<xml_diff>
--- a/Global_M2/TVDataFeed/FinalData/Iraq.xlsx
+++ b/Global_M2/TVDataFeed/FinalData/Iraq.xlsx
@@ -1,40 +1,57 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <workbookPr/>
-  <workbookProtection/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+  <si>
+    <t>Iraq_M2 (IQD)</t>
+  </si>
+  <si>
+    <t>Iraq_FX (USD)</t>
+  </si>
+  <si>
+    <t>Iraq_M2 (USD)</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="yyyy-mm-dd h:mm:ss"/>
-    <numFmt numFmtId="165" formatCode="YYYY-MM-DD HH:MM:SS"/>
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="YYYY-MM-DD HH:MM:SS"/>
   </numFmts>
   <fonts count="2">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b val="1"/>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -49,96 +66,38 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
 </styleSheet>
 </file>
 
@@ -426,3311 +385,3249 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D242"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1">
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>Iraq_M2 (IQD)</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>Iraq_FX (USD)</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>Iraq_M2 (USD)</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="2" t="n">
+    <row r="1" spans="1:4">
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="2">
         <v>37926</v>
       </c>
-      <c r="B2" t="inlineStr"/>
-      <c r="C2" t="n">
+      <c r="C2">
         <v>3.215434083601286</v>
       </c>
-      <c r="D2" t="inlineStr"/>
-    </row>
-    <row r="3">
-      <c r="A3" s="2" t="n">
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="2">
         <v>37956</v>
       </c>
-      <c r="B3" t="n">
+      <c r="B3">
         <v>6953000000000</v>
       </c>
-      <c r="C3" t="inlineStr"/>
-      <c r="D3" t="inlineStr"/>
-    </row>
-    <row r="4">
-      <c r="A4" s="2" t="n">
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="2">
         <v>37987</v>
       </c>
-      <c r="B4" t="n">
+      <c r="B4">
         <v>7445000000000</v>
       </c>
-      <c r="C4" t="inlineStr"/>
-      <c r="D4" t="inlineStr"/>
-    </row>
-    <row r="5">
-      <c r="A5" s="2" t="n">
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" s="2">
         <v>38018</v>
       </c>
-      <c r="B5" t="n">
+      <c r="B5">
         <v>7671000000000</v>
       </c>
-      <c r="C5" t="inlineStr"/>
-      <c r="D5" t="inlineStr"/>
-    </row>
-    <row r="6">
-      <c r="A6" s="2" t="n">
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" s="2">
         <v>38047</v>
       </c>
-      <c r="B6" t="n">
+      <c r="B6">
         <v>7899000000000</v>
       </c>
-      <c r="C6" t="inlineStr"/>
-      <c r="D6" t="inlineStr"/>
-    </row>
-    <row r="7">
-      <c r="A7" s="2" t="n">
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" s="2">
         <v>38078</v>
       </c>
-      <c r="B7" t="n">
+      <c r="B7">
         <v>8261000000000</v>
       </c>
-      <c r="C7" t="inlineStr"/>
-      <c r="D7" t="inlineStr"/>
-    </row>
-    <row r="8">
-      <c r="A8" s="2" t="n">
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" s="2">
         <v>38108</v>
       </c>
-      <c r="B8" t="n">
+      <c r="B8">
         <v>8502000000000</v>
       </c>
-      <c r="C8" t="inlineStr"/>
-      <c r="D8" t="inlineStr"/>
-    </row>
-    <row r="9">
-      <c r="A9" s="2" t="n">
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" s="2">
         <v>38139</v>
       </c>
-      <c r="B9" t="n">
+      <c r="B9">
         <v>9147000000000</v>
       </c>
-      <c r="C9" t="inlineStr"/>
-      <c r="D9" t="inlineStr"/>
-    </row>
-    <row r="10">
-      <c r="A10" s="2" t="n">
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" s="2">
         <v>38169</v>
       </c>
-      <c r="B10" t="n">
+      <c r="B10">
         <v>9367000000000</v>
       </c>
-      <c r="C10" t="inlineStr"/>
-      <c r="D10" t="inlineStr"/>
-    </row>
-    <row r="11">
-      <c r="A11" s="2" t="n">
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" s="2">
         <v>38200</v>
       </c>
-      <c r="B11" t="n">
+      <c r="B11">
         <v>9705000000000</v>
       </c>
-      <c r="C11" t="inlineStr"/>
-      <c r="D11" t="inlineStr"/>
-    </row>
-    <row r="12">
-      <c r="A12" s="2" t="n">
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" s="2">
         <v>38231</v>
       </c>
-      <c r="B12" t="n">
+      <c r="B12">
         <v>9775000000000</v>
       </c>
-      <c r="C12" t="inlineStr"/>
-      <c r="D12" t="inlineStr"/>
-    </row>
-    <row r="13">
-      <c r="A13" s="2" t="n">
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" s="2">
         <v>38261</v>
       </c>
-      <c r="B13" t="n">
+      <c r="B13">
         <v>9588000000000</v>
       </c>
-      <c r="C13" t="inlineStr"/>
-      <c r="D13" t="inlineStr"/>
-    </row>
-    <row r="14">
-      <c r="A14" s="2" t="n">
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" s="2">
         <v>38292</v>
       </c>
-      <c r="B14" t="n">
+      <c r="B14">
         <v>9885000000000</v>
       </c>
-      <c r="C14" t="inlineStr"/>
-      <c r="D14" t="inlineStr"/>
-    </row>
-    <row r="15">
-      <c r="A15" s="2" t="n">
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" s="2">
         <v>38322</v>
       </c>
-      <c r="B15" t="n">
+      <c r="B15">
         <v>12254000000000</v>
       </c>
-      <c r="C15" t="inlineStr"/>
-      <c r="D15" t="inlineStr"/>
-    </row>
-    <row r="16">
-      <c r="A16" s="2" t="n">
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" s="2">
         <v>38353</v>
       </c>
-      <c r="B16" t="n">
+      <c r="B16">
         <v>12474000000000</v>
       </c>
-      <c r="C16" t="inlineStr"/>
-      <c r="D16" t="inlineStr"/>
-    </row>
-    <row r="17">
-      <c r="A17" s="2" t="n">
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" s="2">
         <v>38384</v>
       </c>
-      <c r="B17" t="n">
+      <c r="B17">
         <v>12899000000000</v>
       </c>
-      <c r="C17" t="inlineStr"/>
-      <c r="D17" t="inlineStr"/>
-    </row>
-    <row r="18">
-      <c r="A18" s="2" t="n">
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18" s="2">
         <v>38412</v>
       </c>
-      <c r="B18" t="n">
+      <c r="B18">
         <v>13650000000000</v>
       </c>
-      <c r="C18" t="inlineStr"/>
-      <c r="D18" t="inlineStr"/>
-    </row>
-    <row r="19">
-      <c r="A19" s="2" t="n">
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19" s="2">
         <v>38443</v>
       </c>
-      <c r="B19" t="n">
+      <c r="B19">
         <v>13732000000000</v>
       </c>
-      <c r="C19" t="inlineStr"/>
-      <c r="D19" t="inlineStr"/>
-    </row>
-    <row r="20">
-      <c r="A20" s="2" t="n">
+    </row>
+    <row r="20" spans="1:4">
+      <c r="A20" s="2">
         <v>38473</v>
       </c>
-      <c r="B20" t="n">
+      <c r="B20">
         <v>13888000000000</v>
       </c>
-      <c r="C20" t="inlineStr"/>
-      <c r="D20" t="inlineStr"/>
-    </row>
-    <row r="21">
-      <c r="A21" s="2" t="n">
+    </row>
+    <row r="21" spans="1:4">
+      <c r="A21" s="2">
         <v>38504</v>
       </c>
-      <c r="B21" t="n">
+      <c r="B21">
         <v>13792000000000</v>
       </c>
-      <c r="C21" t="inlineStr"/>
-      <c r="D21" t="inlineStr"/>
-    </row>
-    <row r="22">
-      <c r="A22" s="2" t="n">
+    </row>
+    <row r="22" spans="1:4">
+      <c r="A22" s="2">
         <v>38534</v>
       </c>
-      <c r="B22" t="n">
+      <c r="B22">
         <v>14036000000000</v>
       </c>
-      <c r="C22" t="inlineStr"/>
-      <c r="D22" t="inlineStr"/>
-    </row>
-    <row r="23">
-      <c r="A23" s="2" t="n">
+    </row>
+    <row r="23" spans="1:4">
+      <c r="A23" s="2">
         <v>38565</v>
       </c>
-      <c r="B23" t="n">
+      <c r="B23">
         <v>13278000000000</v>
       </c>
-      <c r="C23" t="inlineStr"/>
-      <c r="D23" t="inlineStr"/>
-    </row>
-    <row r="24">
-      <c r="A24" s="2" t="n">
+    </row>
+    <row r="24" spans="1:4">
+      <c r="A24" s="2">
         <v>38596</v>
       </c>
-      <c r="B24" t="n">
+      <c r="B24">
         <v>13138000000000</v>
       </c>
-      <c r="C24" t="inlineStr"/>
-      <c r="D24" t="inlineStr"/>
-    </row>
-    <row r="25">
-      <c r="A25" s="2" t="n">
+    </row>
+    <row r="25" spans="1:4">
+      <c r="A25" s="2">
         <v>38626</v>
       </c>
-      <c r="B25" t="n">
+      <c r="B25">
         <v>14051000000000</v>
       </c>
-      <c r="C25" t="inlineStr"/>
-      <c r="D25" t="inlineStr"/>
-    </row>
-    <row r="26">
-      <c r="A26" s="2" t="n">
+    </row>
+    <row r="26" spans="1:4">
+      <c r="A26" s="2">
         <v>38657</v>
       </c>
-      <c r="B26" t="n">
+      <c r="B26">
         <v>13272000000000</v>
       </c>
-      <c r="C26" t="inlineStr"/>
-      <c r="D26" t="inlineStr"/>
-    </row>
-    <row r="27">
-      <c r="A27" s="2" t="n">
+    </row>
+    <row r="27" spans="1:4">
+      <c r="A27" s="2">
         <v>38687</v>
       </c>
-      <c r="B27" t="n">
+      <c r="B27">
         <v>14684000000000</v>
       </c>
-      <c r="C27" t="n">
+      <c r="C27">
         <v>0.0006804572672836146</v>
       </c>
-      <c r="D27" t="n">
+      <c r="D27">
         <v>9991834512.792597</v>
       </c>
     </row>
-    <row r="28">
-      <c r="A28" s="2" t="n">
+    <row r="28" spans="1:4">
+      <c r="A28" s="2">
         <v>38718</v>
       </c>
-      <c r="B28" t="n">
+      <c r="B28">
         <v>15267000000000</v>
       </c>
-      <c r="C28" t="n">
+      <c r="C28">
         <v>0.0006804572672836146</v>
       </c>
-      <c r="D28" t="n">
+      <c r="D28">
         <v>10388541099.61894</v>
       </c>
     </row>
-    <row r="29">
-      <c r="A29" s="2" t="n">
+    <row r="29" spans="1:4">
+      <c r="A29" s="2">
         <v>38749</v>
       </c>
-      <c r="B29" t="n">
+      <c r="B29">
         <v>15826000000000</v>
       </c>
-      <c r="C29" t="n">
+      <c r="C29">
         <v>0.0006804572672836146</v>
       </c>
-      <c r="D29" t="n">
+      <c r="D29">
         <v>10768916712.03049</v>
       </c>
     </row>
-    <row r="30">
-      <c r="A30" s="2" t="n">
+    <row r="30" spans="1:4">
+      <c r="A30" s="2">
         <v>38777</v>
       </c>
-      <c r="B30" t="n">
+      <c r="B30">
         <v>16701000000000</v>
       </c>
-      <c r="C30" t="n">
+      <c r="C30">
         <v>0.0006807351940095302</v>
       </c>
-      <c r="D30" t="n">
+      <c r="D30">
         <v>11368958475.15316</v>
       </c>
     </row>
-    <row r="31">
-      <c r="A31" s="2" t="n">
+    <row r="31" spans="1:4">
+      <c r="A31" s="2">
         <v>38808</v>
       </c>
-      <c r="B31" t="n">
+      <c r="B31">
         <v>16842000000000</v>
       </c>
-      <c r="C31" t="n">
+      <c r="C31">
         <v>0.0006807351940095302</v>
       </c>
-      <c r="D31" t="n">
+      <c r="D31">
         <v>11464942137.50851</v>
       </c>
     </row>
-    <row r="32">
-      <c r="A32" s="2" t="n">
+    <row r="32" spans="1:4">
+      <c r="A32" s="2">
         <v>38838</v>
       </c>
-      <c r="B32" t="n">
+      <c r="B32">
         <v>17128000000000</v>
       </c>
-      <c r="C32" t="n">
+      <c r="C32">
         <v>0.0006805035726437564</v>
       </c>
-      <c r="D32" t="n">
+      <c r="D32">
         <v>11655665192.24226</v>
       </c>
     </row>
-    <row r="33">
-      <c r="A33" s="2" t="n">
+    <row r="33" spans="1:4">
+      <c r="A33" s="2">
         <v>38869</v>
       </c>
-      <c r="B33" t="n">
+      <c r="B33">
         <v>17486000000000</v>
       </c>
-      <c r="C33" t="n">
+      <c r="C33">
         <v>0.0006774149844194553</v>
       </c>
-      <c r="D33" t="n">
+      <c r="D33">
         <v>11845278417.5586</v>
       </c>
     </row>
-    <row r="34">
-      <c r="A34" s="2" t="n">
+    <row r="34" spans="1:4">
+      <c r="A34" s="2">
         <v>38899</v>
       </c>
-      <c r="B34" t="n">
+      <c r="B34">
         <v>18820000000000</v>
       </c>
-      <c r="C34" t="n">
+      <c r="C34">
         <v>0.0006775067750677507</v>
       </c>
-      <c r="D34" t="n">
+      <c r="D34">
         <v>12750677506.77507</v>
       </c>
     </row>
-    <row r="35">
-      <c r="A35" s="2" t="n">
+    <row r="35" spans="1:4">
+      <c r="A35" s="2">
         <v>38930</v>
       </c>
-      <c r="B35" t="n">
+      <c r="B35">
         <v>19441000000000</v>
       </c>
-      <c r="C35" t="n">
+      <c r="C35">
         <v>0.0006770480704129993</v>
       </c>
-      <c r="D35" t="n">
+      <c r="D35">
         <v>13162491536.89912</v>
       </c>
     </row>
-    <row r="36">
-      <c r="A36" s="2" t="n">
+    <row r="36" spans="1:4">
+      <c r="A36" s="2">
         <v>38961</v>
       </c>
-      <c r="B36" t="n">
+      <c r="B36">
         <v>19145000000000</v>
       </c>
-      <c r="C36" t="n">
+      <c r="C36">
         <v>0.0006792555359326179</v>
       </c>
-      <c r="D36" t="n">
+      <c r="D36">
         <v>13004347235.42997</v>
       </c>
     </row>
-    <row r="37">
-      <c r="A37" s="2" t="n">
+    <row r="37" spans="1:4">
+      <c r="A37" s="2">
         <v>38991</v>
       </c>
-      <c r="B37" t="n">
+      <c r="B37">
         <v>19538000000000</v>
       </c>
-      <c r="C37" t="n">
+      <c r="C37">
         <v>0.0006790710308298249</v>
       </c>
-      <c r="D37" t="n">
+      <c r="D37">
         <v>13267689800.35312</v>
       </c>
     </row>
-    <row r="38">
-      <c r="A38" s="2" t="n">
+    <row r="38" spans="1:4">
+      <c r="A38" s="2">
         <v>39022</v>
       </c>
-      <c r="B38" t="n">
+      <c r="B38">
         <v>19658000000000</v>
       </c>
-      <c r="C38" t="n">
+      <c r="C38">
         <v>0.0006972528238739366</v>
       </c>
-      <c r="D38" t="n">
+      <c r="D38">
         <v>13706596011.71385</v>
       </c>
     </row>
-    <row r="39">
-      <c r="A39" s="2" t="n">
+    <row r="39" spans="1:4">
+      <c r="A39" s="2">
         <v>39052</v>
       </c>
-      <c r="B39" t="n">
+      <c r="B39">
         <v>21080000000000</v>
       </c>
-      <c r="C39" t="n">
+      <c r="C39">
         <v>0.0007558578987150416</v>
       </c>
-      <c r="D39" t="n">
+      <c r="D39">
         <v>15933484504.91308</v>
       </c>
     </row>
-    <row r="40">
-      <c r="A40" s="2" t="n">
+    <row r="40" spans="1:4">
+      <c r="A40" s="2">
         <v>39083</v>
       </c>
-      <c r="B40" t="n">
+      <c r="B40">
         <v>18329000000000</v>
       </c>
-      <c r="C40" t="n">
+      <c r="C40">
         <v>0.0007748934521503294</v>
       </c>
-      <c r="D40" t="n">
+      <c r="D40">
         <v>14203022084.46339</v>
       </c>
     </row>
-    <row r="41">
-      <c r="A41" s="2" t="n">
+    <row r="41" spans="1:4">
+      <c r="A41" s="2">
         <v>39114</v>
       </c>
-      <c r="B41" t="n">
+      <c r="B41">
         <v>18521000000000</v>
       </c>
-      <c r="C41" t="n">
+      <c r="C41">
         <v>0.0007811279487580066</v>
       </c>
-      <c r="D41" t="n">
+      <c r="D41">
         <v>14467270738.94704</v>
       </c>
     </row>
-    <row r="42">
-      <c r="A42" s="2" t="n">
+    <row r="42" spans="1:4">
+      <c r="A42" s="2">
         <v>39142</v>
       </c>
-      <c r="B42" t="n">
+      <c r="B42">
         <v>18677000000000</v>
       </c>
-      <c r="C42" t="n">
+      <c r="C42">
         <v>0.0007860399308284861</v>
       </c>
-      <c r="D42" t="n">
+      <c r="D42">
         <v>14680867788.08364</v>
       </c>
     </row>
-    <row r="43">
-      <c r="A43" s="2" t="n">
+    <row r="43" spans="1:4">
+      <c r="A43" s="2">
         <v>39173</v>
       </c>
-      <c r="B43" t="n">
+      <c r="B43">
         <v>19144000000000</v>
       </c>
-      <c r="C43" t="n">
+      <c r="C43">
         <v>0.000787897888433659</v>
       </c>
-      <c r="D43" t="n">
+      <c r="D43">
         <v>15083517176.17397</v>
       </c>
     </row>
-    <row r="44">
-      <c r="A44" s="2" t="n">
+    <row r="44" spans="1:4">
+      <c r="A44" s="2">
         <v>39203</v>
       </c>
-      <c r="B44" t="n">
+      <c r="B44">
         <v>18148000000000</v>
       </c>
-      <c r="C44" t="n">
+      <c r="C44">
         <v>0.0007952286282306163</v>
       </c>
-      <c r="D44" t="n">
+      <c r="D44">
         <v>14431809145.12922</v>
       </c>
     </row>
-    <row r="45">
-      <c r="A45" s="2" t="n">
+    <row r="45" spans="1:4">
+      <c r="A45" s="2">
         <v>39234</v>
       </c>
-      <c r="B45" t="n">
+      <c r="B45">
         <v>18791000000000</v>
       </c>
-      <c r="C45" t="n">
+      <c r="C45">
         <v>0.0007994244144216163</v>
       </c>
-      <c r="D45" t="n">
+      <c r="D45">
         <v>15021984171.39659</v>
       </c>
     </row>
-    <row r="46">
-      <c r="A46" s="2" t="n">
+    <row r="46" spans="1:4">
+      <c r="A46" s="2">
         <v>39264</v>
       </c>
-      <c r="B46" t="n">
+      <c r="B46">
         <v>19577000000000</v>
       </c>
-      <c r="C46" t="n">
+      <c r="C46">
         <v>0.0008058017727639</v>
       </c>
-      <c r="D46" t="n">
+      <c r="D46">
         <v>15775181305.39887</v>
       </c>
     </row>
-    <row r="47">
-      <c r="A47" s="2" t="n">
+    <row r="47" spans="1:4">
+      <c r="A47" s="2">
         <v>39295</v>
       </c>
-      <c r="B47" t="n">
+      <c r="B47">
         <v>20302000000000</v>
       </c>
-      <c r="C47" t="n">
+      <c r="C47">
         <v>0.0008087343307723412</v>
       </c>
-      <c r="D47" t="n">
+      <c r="D47">
         <v>16418924383.34007</v>
       </c>
     </row>
-    <row r="48">
-      <c r="A48" s="2" t="n">
+    <row r="48" spans="1:4">
+      <c r="A48" s="2">
         <v>39326</v>
       </c>
-      <c r="B48" t="n">
+      <c r="B48">
         <v>22525000000000</v>
       </c>
-      <c r="C48" t="n">
+      <c r="C48">
         <v>0.0008113590263691683</v>
       </c>
-      <c r="D48" t="n">
+      <c r="D48">
         <v>18275862068.96552</v>
       </c>
     </row>
-    <row r="49">
-      <c r="A49" s="2" t="n">
+    <row r="49" spans="1:4">
+      <c r="A49" s="2">
         <v>39356</v>
       </c>
-      <c r="B49" t="n">
+      <c r="B49">
         <v>23445000000000</v>
       </c>
-      <c r="C49" t="n">
+      <c r="C49">
         <v>0.0008134710811030668</v>
       </c>
-      <c r="D49" t="n">
+      <c r="D49">
         <v>19071829496.4614</v>
       </c>
     </row>
-    <row r="50">
-      <c r="A50" s="2" t="n">
+    <row r="50" spans="1:4">
+      <c r="A50" s="2">
         <v>39387</v>
       </c>
-      <c r="B50" t="n">
+      <c r="B50">
         <v>23523000000000</v>
       </c>
-      <c r="C50" t="n">
+      <c r="C50">
         <v>0.0008185985592665358</v>
       </c>
-      <c r="D50" t="n">
+      <c r="D50">
         <v>19255893909.62672</v>
       </c>
     </row>
-    <row r="51">
-      <c r="A51" s="2" t="n">
+    <row r="51" spans="1:4">
+      <c r="A51" s="2">
         <v>39417</v>
       </c>
-      <c r="B51" t="n">
+      <c r="B51">
         <v>26956000000000</v>
       </c>
-      <c r="C51" t="n">
+      <c r="C51">
         <v>0.0008239947264337509</v>
       </c>
-      <c r="D51" t="n">
+      <c r="D51">
         <v>22211601845.74819</v>
       </c>
     </row>
-    <row r="52">
-      <c r="A52" s="2" t="n">
+    <row r="52" spans="1:4">
+      <c r="A52" s="2">
         <v>39448</v>
       </c>
-      <c r="B52" t="n">
+      <c r="B52">
         <v>27037000000000</v>
       </c>
-      <c r="C52" t="n">
+      <c r="C52">
         <v>0.0008254911672445104</v>
       </c>
-      <c r="D52" t="n">
+      <c r="D52">
         <v>22318804688.78983</v>
       </c>
     </row>
-    <row r="53">
-      <c r="A53" s="2" t="n">
+    <row r="53" spans="1:4">
+      <c r="A53" s="2">
         <v>39479</v>
       </c>
-      <c r="B53" t="n">
+      <c r="B53">
         <v>25349000000000</v>
       </c>
-      <c r="C53" t="n">
+      <c r="C53">
         <v>0.0008275405494869248</v>
       </c>
-      <c r="D53" t="n">
+      <c r="D53">
         <v>20977325388.94406</v>
       </c>
     </row>
-    <row r="54">
-      <c r="A54" s="2" t="n">
+    <row r="54" spans="1:4">
+      <c r="A54" s="2">
         <v>39508</v>
       </c>
-      <c r="B54" t="n">
+      <c r="B54">
         <v>25911000000000</v>
       </c>
-      <c r="C54" t="n">
+      <c r="C54">
         <v>0.0008305647840531562</v>
       </c>
-      <c r="D54" t="n">
+      <c r="D54">
         <v>21520764119.60133</v>
       </c>
     </row>
-    <row r="55">
-      <c r="A55" s="2" t="n">
+    <row r="55" spans="1:4">
+      <c r="A55" s="2">
         <v>39539</v>
       </c>
-      <c r="B55" t="n">
+      <c r="B55">
         <v>26081000000000</v>
       </c>
-      <c r="C55" t="n">
+      <c r="C55">
         <v>0.0008314625426124552</v>
       </c>
-      <c r="D55" t="n">
+      <c r="D55">
         <v>21685374573.87545</v>
       </c>
     </row>
-    <row r="56">
-      <c r="A56" s="2" t="n">
+    <row r="56" spans="1:4">
+      <c r="A56" s="2">
         <v>39569</v>
       </c>
-      <c r="B56" t="n">
+      <c r="B56">
         <v>26580000000000</v>
       </c>
-      <c r="C56" t="n">
+      <c r="C56">
         <v>0.0008336112037345783</v>
       </c>
-      <c r="D56" t="n">
+      <c r="D56">
         <v>22157385795.26509</v>
       </c>
     </row>
-    <row r="57">
-      <c r="A57" s="2" t="n">
+    <row r="57" spans="1:4">
+      <c r="A57" s="2">
         <v>39600</v>
       </c>
-      <c r="B57" t="n">
+      <c r="B57">
         <v>28481000000000</v>
       </c>
-      <c r="C57" t="n">
+      <c r="C57">
         <v>0.00083633018315631</v>
       </c>
-      <c r="D57" t="n">
+      <c r="D57">
         <v>23819519946.47486</v>
       </c>
     </row>
-    <row r="58">
-      <c r="A58" s="2" t="n">
+    <row r="58" spans="1:4">
+      <c r="A58" s="2">
         <v>39630</v>
       </c>
-      <c r="B58" t="n">
+      <c r="B58">
         <v>29825000000000</v>
       </c>
-      <c r="C58" t="n">
+      <c r="C58">
         <v>0.0008676036786395975</v>
       </c>
-      <c r="D58" t="n">
+      <c r="D58">
         <v>25876279715.42599</v>
       </c>
     </row>
-    <row r="59">
-      <c r="A59" s="2" t="n">
+    <row r="59" spans="1:4">
+      <c r="A59" s="2">
         <v>39661</v>
       </c>
-      <c r="B59" t="n">
+      <c r="B59">
         <v>30880000000000</v>
       </c>
-      <c r="C59" t="n">
+      <c r="C59">
         <v>0.0008456659619450317</v>
       </c>
-      <c r="D59" t="n">
+      <c r="D59">
         <v>26114164904.86258</v>
       </c>
     </row>
-    <row r="60">
-      <c r="A60" s="2" t="n">
+    <row r="60" spans="1:4">
+      <c r="A60" s="2">
         <v>39692</v>
       </c>
-      <c r="B60" t="n">
+      <c r="B60">
         <v>32536000000000</v>
       </c>
-      <c r="C60" t="n">
+      <c r="C60">
         <v>0.0008491847826086957</v>
       </c>
-      <c r="D60" t="n">
+      <c r="D60">
         <v>27629076086.95652</v>
       </c>
     </row>
-    <row r="61">
-      <c r="A61" s="2" t="n">
+    <row r="61" spans="1:4">
+      <c r="A61" s="2">
         <v>39722</v>
       </c>
-      <c r="B61" t="n">
+      <c r="B61">
         <v>31295000000000</v>
       </c>
-      <c r="C61" t="n">
+      <c r="C61">
         <v>0.0008542627712284299</v>
       </c>
-      <c r="D61" t="n">
+      <c r="D61">
         <v>26734153425.59372</v>
       </c>
     </row>
-    <row r="62">
-      <c r="A62" s="2" t="n">
+    <row r="62" spans="1:4">
+      <c r="A62" s="2">
         <v>39753</v>
       </c>
-      <c r="B62" t="n">
+      <c r="B62">
         <v>33580000000000</v>
       </c>
-      <c r="C62" t="n">
+      <c r="C62">
         <v>0.0008542627712284299</v>
       </c>
-      <c r="D62" t="n">
+      <c r="D62">
         <v>28686143857.85068</v>
       </c>
     </row>
-    <row r="63">
-      <c r="A63" s="2" t="n">
+    <row r="63" spans="1:4">
+      <c r="A63" s="2">
         <v>39783</v>
       </c>
-      <c r="B63" t="n">
+      <c r="B63">
         <v>34920000000000</v>
       </c>
-      <c r="C63" t="n">
+      <c r="C63">
         <v>0.0008653513326410524</v>
       </c>
-      <c r="D63" t="n">
+      <c r="D63">
         <v>30218068535.82555</v>
       </c>
     </row>
-    <row r="64">
-      <c r="A64" s="2" t="n">
+    <row r="64" spans="1:4">
+      <c r="A64" s="2">
         <v>39814</v>
       </c>
-      <c r="B64" t="n">
+      <c r="B64">
         <v>36187000000000</v>
       </c>
-      <c r="C64" t="n">
+      <c r="C64">
         <v>0.000869187309865276</v>
       </c>
-      <c r="D64" t="n">
+      <c r="D64">
         <v>31453281182.09474</v>
       </c>
     </row>
-    <row r="65">
-      <c r="A65" s="2" t="n">
+    <row r="65" spans="1:4">
+      <c r="A65" s="2">
         <v>39845</v>
       </c>
-      <c r="B65" t="n">
+      <c r="B65">
         <v>37659000000000</v>
       </c>
-      <c r="C65" t="n">
+      <c r="C65">
         <v>0.0008714596949891067</v>
       </c>
-      <c r="D65" t="n">
+      <c r="D65">
         <v>32818300653.59477</v>
       </c>
     </row>
-    <row r="66">
-      <c r="A66" s="2" t="n">
+    <row r="66" spans="1:4">
+      <c r="A66" s="2">
         <v>39873</v>
       </c>
-      <c r="B66" t="n">
+      <c r="B66">
         <v>36973000000000</v>
       </c>
-      <c r="C66" t="n">
+      <c r="C66">
         <v>0.0008654262224145391</v>
       </c>
-      <c r="D66" t="n">
+      <c r="D66">
         <v>31997403721.33276</v>
       </c>
     </row>
-    <row r="67">
-      <c r="A67" s="2" t="n">
+    <row r="67" spans="1:4">
+      <c r="A67" s="2">
         <v>39904</v>
       </c>
-      <c r="B67" t="n">
+      <c r="B67">
         <v>36721000000000</v>
       </c>
-      <c r="C67" t="n">
+      <c r="C67">
         <v>0.0008653513326410524</v>
       </c>
-      <c r="D67" t="n">
+      <c r="D67">
         <v>31776566285.91209</v>
       </c>
     </row>
-    <row r="68">
-      <c r="A68" s="2" t="n">
+    <row r="68" spans="1:4">
+      <c r="A68" s="2">
         <v>39934</v>
       </c>
-      <c r="B68" t="n">
+      <c r="B68">
         <v>36957000000000</v>
       </c>
-      <c r="C68" t="n">
+      <c r="C68">
         <v>0.0008653513326410524</v>
       </c>
-      <c r="D68" t="n">
+      <c r="D68">
         <v>31980789200.41537</v>
       </c>
     </row>
-    <row r="69">
-      <c r="A69" s="2" t="n">
+    <row r="69" spans="1:4">
+      <c r="A69" s="2">
         <v>39965</v>
       </c>
-      <c r="B69" t="n">
+      <c r="B69">
         <v>37811000000000</v>
       </c>
-      <c r="C69" t="n">
+      <c r="C69">
         <v>0.0008653887759075765</v>
       </c>
-      <c r="D69" t="n">
+      <c r="D69">
         <v>32721215005.84137</v>
       </c>
     </row>
-    <row r="70">
-      <c r="A70" s="2" t="n">
+    <row r="70" spans="1:4">
+      <c r="A70" s="2">
         <v>39995</v>
       </c>
-      <c r="B70" t="n">
+      <c r="B70">
         <v>38807000000000</v>
       </c>
-      <c r="C70" t="n">
+      <c r="C70">
         <v>0.0008654262224145391</v>
       </c>
-      <c r="D70" t="n">
+      <c r="D70">
         <v>33584595413.24102</v>
       </c>
     </row>
-    <row r="71">
-      <c r="A71" s="2" t="n">
+    <row r="71" spans="1:4">
+      <c r="A71" s="2">
         <v>40026</v>
       </c>
-      <c r="B71" t="n">
+      <c r="B71">
         <v>39690000000000</v>
       </c>
-      <c r="C71" t="n">
+      <c r="C71">
         <v>0.000869187309865276</v>
       </c>
-      <c r="D71" t="n">
+      <c r="D71">
         <v>34498044328.5528</v>
       </c>
     </row>
-    <row r="72">
-      <c r="A72" s="2" t="n">
+    <row r="72" spans="1:4">
+      <c r="A72" s="2">
         <v>40057</v>
       </c>
-      <c r="B72" t="n">
+      <c r="B72">
         <v>42983000000000</v>
       </c>
-      <c r="C72" t="n">
+      <c r="C72">
         <v>0.000869187309865276</v>
       </c>
-      <c r="D72" t="n">
+      <c r="D72">
         <v>37360278139.93916</v>
       </c>
     </row>
-    <row r="73">
-      <c r="A73" s="2" t="n">
+    <row r="73" spans="1:4">
+      <c r="A73" s="2">
         <v>40087</v>
       </c>
-      <c r="B73" t="n">
+      <c r="B73">
         <v>42921000000000</v>
       </c>
-      <c r="C73" t="n">
+      <c r="C73">
         <v>0.000869187309865276</v>
       </c>
-      <c r="D73" t="n">
+      <c r="D73">
         <v>37306388526.72751</v>
       </c>
     </row>
-    <row r="74">
-      <c r="A74" s="2" t="n">
+    <row r="74" spans="1:4">
+      <c r="A74" s="2">
         <v>40118</v>
       </c>
-      <c r="B74" t="n">
+      <c r="B74">
         <v>43814000000000</v>
       </c>
-      <c r="C74" t="n">
+      <c r="C74">
         <v>0.0008691495371778715</v>
       </c>
-      <c r="D74" t="n">
+      <c r="D74">
         <v>38080917821.91126</v>
       </c>
     </row>
-    <row r="75">
-      <c r="A75" s="2" t="n">
+    <row r="75" spans="1:4">
+      <c r="A75" s="2">
         <v>40148</v>
       </c>
-      <c r="B75" t="n">
+      <c r="B75">
         <v>45438000000000</v>
       </c>
-      <c r="C75" t="n">
+      <c r="C75">
         <v>0.000869187309865276</v>
       </c>
-      <c r="D75" t="n">
+      <c r="D75">
         <v>39494132985.65841</v>
       </c>
     </row>
-    <row r="76">
-      <c r="A76" s="2" t="n">
+    <row r="76" spans="1:4">
+      <c r="A76" s="2">
         <v>40179</v>
       </c>
-      <c r="B76" t="n">
+      <c r="B76">
         <v>46211000000000</v>
       </c>
-      <c r="C76" t="n">
+      <c r="C76">
         <v>0.0008691495371778715</v>
       </c>
-      <c r="D76" t="n">
+      <c r="D76">
         <v>40164269262.52662</v>
       </c>
     </row>
-    <row r="77">
-      <c r="A77" s="2" t="n">
+    <row r="77" spans="1:4">
+      <c r="A77" s="2">
         <v>40210</v>
       </c>
-      <c r="B77" t="n">
+      <c r="B77">
         <v>47666000000000</v>
       </c>
-      <c r="C77" t="n">
+      <c r="C77">
         <v>0.0008595495960116898</v>
       </c>
-      <c r="D77" t="n">
+      <c r="D77">
         <v>40971291043.4932</v>
       </c>
     </row>
-    <row r="78">
-      <c r="A78" s="2" t="n">
+    <row r="78" spans="1:4">
+      <c r="A78" s="2">
         <v>40238</v>
       </c>
-      <c r="B78" t="n">
+      <c r="B78">
         <v>49265000000000</v>
       </c>
-      <c r="C78" t="n">
+      <c r="C78">
         <v>0.0008579640513062503</v>
       </c>
-      <c r="D78" t="n">
+      <c r="D78">
         <v>42267598987.60242</v>
       </c>
     </row>
-    <row r="79">
-      <c r="A79" s="2" t="n">
+    <row r="79" spans="1:4">
+      <c r="A79" s="2">
         <v>40269</v>
       </c>
-      <c r="B79" t="n">
+      <c r="B79">
         <v>51224000000000</v>
       </c>
-      <c r="C79" t="n">
+      <c r="C79">
         <v>0.0008583690987124463</v>
       </c>
-      <c r="D79" t="n">
+      <c r="D79">
         <v>43969098712.44635</v>
       </c>
     </row>
-    <row r="80">
-      <c r="A80" s="2" t="n">
+    <row r="80" spans="1:4">
+      <c r="A80" s="2">
         <v>40299</v>
       </c>
-      <c r="B80" t="n">
+      <c r="B80">
         <v>53051000000000</v>
       </c>
-      <c r="C80" t="n">
+      <c r="C80">
         <v>0.000858000858000858</v>
       </c>
-      <c r="D80" t="n">
+      <c r="D80">
         <v>45517803517.80352</v>
       </c>
     </row>
-    <row r="81">
-      <c r="A81" s="2" t="n">
+    <row r="81" spans="1:4">
+      <c r="A81" s="2">
         <v>40330</v>
       </c>
-      <c r="B81" t="n">
+      <c r="B81">
         <v>55851000000000</v>
       </c>
-      <c r="C81" t="n">
+      <c r="C81">
         <v>0.000858000858000858</v>
       </c>
-      <c r="D81" t="n">
+      <c r="D81">
         <v>47920205920.20592</v>
       </c>
     </row>
-    <row r="82">
-      <c r="A82" s="2" t="n">
+    <row r="82" spans="1:4">
+      <c r="A82" s="2">
         <v>40360</v>
       </c>
-      <c r="B82" t="n">
+      <c r="B82">
         <v>55874000000000</v>
       </c>
-      <c r="C82" t="n">
+      <c r="C82">
         <v>0.0008583690987124463</v>
       </c>
-      <c r="D82" t="n">
+      <c r="D82">
         <v>47960515021.45923</v>
       </c>
     </row>
-    <row r="83">
-      <c r="A83" s="2" t="n">
+    <row r="83" spans="1:4">
+      <c r="A83" s="2">
         <v>40391</v>
       </c>
-      <c r="B83" t="n">
+      <c r="B83">
         <v>56388000000000</v>
       </c>
-      <c r="C83" t="n">
+      <c r="C83">
         <v>0.0008557980316645272</v>
       </c>
-      <c r="D83" t="n">
+      <c r="D83">
         <v>48256739409.49936</v>
       </c>
     </row>
-    <row r="84">
-      <c r="A84" s="2" t="n">
+    <row r="84" spans="1:4">
+      <c r="A84" s="2">
         <v>40422</v>
       </c>
-      <c r="B84" t="n">
+      <c r="B84">
         <v>56213000000000</v>
       </c>
-      <c r="C84" t="n">
+      <c r="C84">
         <v>0.0008571183680466272</v>
       </c>
-      <c r="D84" t="n">
+      <c r="D84">
         <v>48181194823.00505</v>
       </c>
     </row>
-    <row r="85">
-      <c r="A85" s="2" t="n">
+    <row r="85" spans="1:4">
+      <c r="A85" s="2">
         <v>40452</v>
       </c>
-      <c r="B85" t="n">
+      <c r="B85">
         <v>57299000000000</v>
       </c>
-      <c r="C85" t="n">
+      <c r="C85">
         <v>0.0008572285800008573</v>
       </c>
-      <c r="D85" t="n">
+      <c r="D85">
         <v>49118340405.46912</v>
       </c>
     </row>
-    <row r="86">
-      <c r="A86" s="2" t="n">
+    <row r="86" spans="1:4">
+      <c r="A86" s="2">
         <v>40483</v>
       </c>
-      <c r="B86" t="n">
+      <c r="B86">
         <v>58201000000000</v>
       </c>
-      <c r="C86" t="n">
+      <c r="C86">
         <v>0.0008583690987124463</v>
       </c>
-      <c r="D86" t="n">
+      <c r="D86">
         <v>49957939914.16309</v>
       </c>
     </row>
-    <row r="87">
-      <c r="A87" s="2" t="n">
+    <row r="87" spans="1:4">
+      <c r="A87" s="2">
         <v>40513</v>
       </c>
-      <c r="B87" t="n">
+      <c r="B87">
         <v>60386000000000</v>
       </c>
-      <c r="C87" t="n">
+      <c r="C87">
         <v>0.000856898029134533</v>
       </c>
-      <c r="D87" t="n">
+      <c r="D87">
         <v>51744644387.31791</v>
       </c>
     </row>
-    <row r="88">
-      <c r="A88" s="2" t="n">
+    <row r="88" spans="1:4">
+      <c r="A88" s="2">
         <v>40544</v>
       </c>
-      <c r="B88" t="n">
+      <c r="B88">
         <v>60809000000000</v>
       </c>
-      <c r="C88" t="n">
+      <c r="C88">
         <v>0.0008507018290089324</v>
       </c>
-      <c r="D88" t="n">
+      <c r="D88">
         <v>51730327520.20417</v>
       </c>
     </row>
-    <row r="89">
-      <c r="A89" s="2" t="n">
+    <row r="89" spans="1:4">
+      <c r="A89" s="2">
         <v>40575</v>
       </c>
-      <c r="B89" t="n">
+      <c r="B89">
         <v>59740000000000</v>
       </c>
-      <c r="C89" t="n">
+      <c r="C89">
         <v>0.0008507018290089324</v>
       </c>
-      <c r="D89" t="n">
+      <c r="D89">
         <v>50820927264.99362</v>
       </c>
     </row>
-    <row r="90">
-      <c r="A90" s="2" t="n">
+    <row r="90" spans="1:4">
+      <c r="A90" s="2">
         <v>40603</v>
       </c>
-      <c r="B90" t="n">
+      <c r="B90">
         <v>58453000000000</v>
       </c>
-      <c r="C90" t="n">
+      <c r="C90">
         <v>0.0008507018290089324</v>
       </c>
-      <c r="D90" t="n">
+      <c r="D90">
         <v>49726074011.05913</v>
       </c>
     </row>
-    <row r="91">
-      <c r="A91" s="2" t="n">
+    <row r="91" spans="1:4">
+      <c r="A91" s="2">
         <v>40634</v>
       </c>
-      <c r="B91" t="n">
+      <c r="B91">
         <v>59265000000000</v>
       </c>
-      <c r="C91" t="n">
+      <c r="C91">
         <v>0.0008583690987124463</v>
       </c>
-      <c r="D91" t="n">
+      <c r="D91">
         <v>50871244635.19313</v>
       </c>
     </row>
-    <row r="92">
-      <c r="A92" s="2" t="n">
+    <row r="92" spans="1:4">
+      <c r="A92" s="2">
         <v>40664</v>
       </c>
-      <c r="B92" t="n">
+      <c r="B92">
         <v>59602000000000</v>
       </c>
-      <c r="C92" t="n">
+      <c r="C92">
         <v>0.000858000858000858</v>
       </c>
-      <c r="D92" t="n">
+      <c r="D92">
         <v>51138567138.56714</v>
       </c>
     </row>
-    <row r="93">
-      <c r="A93" s="2" t="n">
+    <row r="93" spans="1:4">
+      <c r="A93" s="2">
         <v>40695</v>
       </c>
-      <c r="B93" t="n">
+      <c r="B93">
         <v>62322000000000</v>
       </c>
-      <c r="C93" t="n">
+      <c r="C93">
         <v>0.0008576329331046312</v>
       </c>
-      <c r="D93" t="n">
+      <c r="D93">
         <v>53449399656.94682</v>
       </c>
     </row>
-    <row r="94">
-      <c r="A94" s="2" t="n">
+    <row r="94" spans="1:4">
+      <c r="A94" s="2">
         <v>40725</v>
       </c>
-      <c r="B94" t="n">
+      <c r="B94">
         <v>64438000000000</v>
       </c>
-      <c r="C94" t="n">
+      <c r="C94">
         <v>0.0008572285800008573</v>
       </c>
-      <c r="D94" t="n">
+      <c r="D94">
         <v>55238095238.09524</v>
       </c>
     </row>
-    <row r="95">
-      <c r="A95" s="2" t="n">
+    <row r="95" spans="1:4">
+      <c r="A95" s="2">
         <v>40756</v>
       </c>
-      <c r="B95" t="n">
+      <c r="B95">
         <v>65125000000000</v>
       </c>
-      <c r="C95" t="n">
+      <c r="C95">
         <v>0.0008572653236176596</v>
       </c>
-      <c r="D95" t="n">
+      <c r="D95">
         <v>55829404200.60008</v>
       </c>
     </row>
-    <row r="96">
-      <c r="A96" s="2" t="n">
+    <row r="96" spans="1:4">
+      <c r="A96" s="2">
         <v>40787</v>
       </c>
-      <c r="B96" t="n">
+      <c r="B96">
         <v>65111000000000</v>
       </c>
-      <c r="C96" t="n">
+      <c r="C96">
         <v>0.0008572653236176596</v>
       </c>
-      <c r="D96" t="n">
+      <c r="D96">
         <v>55817402486.06944</v>
       </c>
     </row>
-    <row r="97">
-      <c r="A97" s="2" t="n">
+    <row r="97" spans="1:4">
+      <c r="A97" s="2">
         <v>40817</v>
       </c>
-      <c r="B97" t="n">
+      <c r="B97">
         <v>67148000000000</v>
       </c>
-      <c r="C97" t="n">
+      <c r="C97">
         <v>0.0008565310492505353</v>
       </c>
-      <c r="D97" t="n">
+      <c r="D97">
         <v>57514346895.07494</v>
       </c>
     </row>
-    <row r="98">
-      <c r="A98" s="2" t="n">
+    <row r="98" spans="1:4">
+      <c r="A98" s="2">
         <v>40848</v>
       </c>
-      <c r="B98" t="n">
+      <c r="B98">
         <v>68973000000000</v>
       </c>
-      <c r="C98" t="n">
+      <c r="C98">
         <v>0.000856898029134533</v>
       </c>
-      <c r="D98" t="n">
+      <c r="D98">
         <v>59102827763.49615</v>
       </c>
     </row>
-    <row r="99">
-      <c r="A99" s="2" t="n">
+    <row r="99" spans="1:4">
+      <c r="A99" s="2">
         <v>40878</v>
       </c>
-      <c r="B99" t="n">
+      <c r="B99">
         <v>72178000000000</v>
       </c>
-      <c r="C99" t="n">
+      <c r="C99">
         <v>0.0008550662676357417</v>
       </c>
-      <c r="D99" t="n">
+      <c r="D99">
         <v>61716973065.41257</v>
       </c>
     </row>
-    <row r="100">
-      <c r="A100" s="2" t="n">
+    <row r="100" spans="1:4">
+      <c r="A100" s="2">
         <v>40909</v>
       </c>
-      <c r="B100" t="n">
+      <c r="B100">
         <v>71626700000000</v>
       </c>
-      <c r="C100" t="n">
+      <c r="C100">
         <v>0.0008598452278589854</v>
       </c>
-      <c r="D100" t="n">
+      <c r="D100">
         <v>61587876182.28719</v>
       </c>
     </row>
-    <row r="101">
-      <c r="A101" s="2" t="n">
+    <row r="101" spans="1:4">
+      <c r="A101" s="2">
         <v>40940</v>
       </c>
-      <c r="B101" t="n">
+      <c r="B101">
         <v>72389800000000</v>
       </c>
-      <c r="C101" t="n">
+      <c r="C101">
         <v>0.0008598452278589854</v>
       </c>
-      <c r="D101" t="n">
+      <c r="D101">
         <v>62244024075.66638</v>
       </c>
     </row>
-    <row r="102">
-      <c r="A102" s="2" t="n">
+    <row r="102" spans="1:4">
+      <c r="A102" s="2">
         <v>40969</v>
       </c>
-      <c r="B102" t="n">
+      <c r="B102">
         <v>73592600000000</v>
       </c>
-      <c r="C102" t="n">
+      <c r="C102">
         <v>0.000858000858000858</v>
       </c>
-      <c r="D102" t="n">
+      <c r="D102">
         <v>63142513942.51395</v>
       </c>
     </row>
-    <row r="103">
-      <c r="A103" s="2" t="n">
+    <row r="103" spans="1:4">
+      <c r="A103" s="2">
         <v>41000</v>
       </c>
-      <c r="B103" t="n">
+      <c r="B103">
         <v>75216000000000</v>
       </c>
-      <c r="C103" t="n">
+      <c r="C103">
         <v>0.0008614748449345279</v>
       </c>
-      <c r="D103" t="n">
+      <c r="D103">
         <v>64796691936.59545</v>
       </c>
     </row>
-    <row r="104">
-      <c r="A104" s="2" t="n">
+    <row r="104" spans="1:4">
+      <c r="A104" s="2">
         <v>41030</v>
       </c>
-      <c r="B104" t="n">
+      <c r="B104">
         <v>73207900000000</v>
       </c>
-      <c r="C104" t="n">
+      <c r="C104">
         <v>0.0008605851979345956</v>
       </c>
-      <c r="D104" t="n">
+      <c r="D104">
         <v>63001635111.87608</v>
       </c>
     </row>
-    <row r="105">
-      <c r="A105" s="2" t="n">
+    <row r="105" spans="1:4">
+      <c r="A105" s="2">
         <v>41061</v>
       </c>
-      <c r="B105" t="n">
+      <c r="B105">
         <v>72682900000000</v>
       </c>
-      <c r="C105" t="n">
+      <c r="C105">
         <v>0.000858000858000858</v>
       </c>
-      <c r="D105" t="n">
+      <c r="D105">
         <v>62361990561.99056</v>
       </c>
     </row>
-    <row r="106">
-      <c r="A106" s="2" t="n">
+    <row r="106" spans="1:4">
+      <c r="A106" s="2">
         <v>41091</v>
       </c>
-      <c r="B106" t="n">
+      <c r="B106">
         <v>72968200000000</v>
       </c>
-      <c r="C106" t="n">
+      <c r="C106">
         <v>0.0008583690987124463</v>
       </c>
-      <c r="D106" t="n">
+      <c r="D106">
         <v>62633648068.66953</v>
       </c>
     </row>
-    <row r="107">
-      <c r="A107" s="2" t="n">
+    <row r="107" spans="1:4">
+      <c r="A107" s="2">
         <v>41122</v>
       </c>
-      <c r="B107" t="n">
+      <c r="B107">
         <v>73768600000000</v>
       </c>
-      <c r="C107" t="n">
+      <c r="C107">
         <v>0.0008583690987124463</v>
       </c>
-      <c r="D107" t="n">
+      <c r="D107">
         <v>63320686695.27897</v>
       </c>
     </row>
-    <row r="108">
-      <c r="A108" s="2" t="n">
+    <row r="108" spans="1:4">
+      <c r="A108" s="2">
         <v>41153</v>
       </c>
-      <c r="B108" t="n">
+      <c r="B108">
         <v>73543300000000</v>
       </c>
-      <c r="C108" t="n">
+      <c r="C108">
         <v>0.000858000858000858</v>
       </c>
-      <c r="D108" t="n">
+      <c r="D108">
         <v>63100214500.2145</v>
       </c>
     </row>
-    <row r="109">
-      <c r="A109" s="2" t="n">
+    <row r="109" spans="1:4">
+      <c r="A109" s="2">
         <v>41183</v>
       </c>
-      <c r="B109" t="n">
+      <c r="B109">
         <v>74254400000000</v>
       </c>
-      <c r="C109" t="n">
+      <c r="C109">
         <v>0.0008583690987124463</v>
       </c>
-      <c r="D109" t="n">
+      <c r="D109">
         <v>63737682403.43347</v>
       </c>
     </row>
-    <row r="110">
-      <c r="A110" s="2" t="n">
+    <row r="110" spans="1:4">
+      <c r="A110" s="2">
         <v>41214</v>
       </c>
-      <c r="B110" t="n">
+      <c r="B110">
         <v>74863700000000</v>
       </c>
-      <c r="C110" t="n">
+      <c r="C110">
         <v>0.0008598452278589854</v>
       </c>
-      <c r="D110" t="n">
+      <c r="D110">
         <v>64371195184.86672</v>
       </c>
     </row>
-    <row r="111">
-      <c r="A111" s="2" t="n">
+    <row r="111" spans="1:4">
+      <c r="A111" s="2">
         <v>41244</v>
       </c>
-      <c r="B111" t="n">
+      <c r="B111">
         <v>77187500000000</v>
       </c>
-      <c r="C111" t="n">
+      <c r="C111">
         <v>0.0008598452278589854</v>
       </c>
-      <c r="D111" t="n">
+      <c r="D111">
         <v>66369303525.36543</v>
       </c>
     </row>
-    <row r="112">
-      <c r="A112" s="2" t="n">
+    <row r="112" spans="1:4">
+      <c r="A112" s="2">
         <v>41275</v>
       </c>
-      <c r="B112" t="n">
+      <c r="B112">
         <v>77336800000000</v>
       </c>
-      <c r="C112" t="n">
+      <c r="C112">
         <v>0.0008598452278589854</v>
       </c>
-      <c r="D112" t="n">
+      <c r="D112">
         <v>66497678417.88478</v>
       </c>
     </row>
-    <row r="113">
-      <c r="A113" s="2" t="n">
+    <row r="113" spans="1:4">
+      <c r="A113" s="2">
         <v>41306</v>
       </c>
-      <c r="B113" t="n">
+      <c r="B113">
         <v>78554700000000</v>
       </c>
-      <c r="C113" t="n">
+      <c r="C113">
         <v>0.0008613264427217916</v>
       </c>
-      <c r="D113" t="n">
+      <c r="D113">
         <v>67661240310.07752</v>
       </c>
     </row>
-    <row r="114">
-      <c r="A114" s="2" t="n">
+    <row r="114" spans="1:4">
+      <c r="A114" s="2">
         <v>41334</v>
       </c>
-      <c r="B114" t="n">
+      <c r="B114">
         <v>80238400000000</v>
       </c>
-      <c r="C114" t="n">
+      <c r="C114">
         <v>0.0008620689655172414</v>
       </c>
-      <c r="D114" t="n">
+      <c r="D114">
         <v>69171034482.75862</v>
       </c>
     </row>
-    <row r="115">
-      <c r="A115" s="2" t="n">
+    <row r="115" spans="1:4">
+      <c r="A115" s="2">
         <v>41365</v>
       </c>
-      <c r="B115" t="n">
+      <c r="B115">
         <v>83367600000000</v>
       </c>
-      <c r="C115" t="n">
+      <c r="C115">
         <v>0.000864304235090752</v>
       </c>
-      <c r="D115" t="n">
+      <c r="D115">
         <v>72054969749.35178</v>
       </c>
     </row>
-    <row r="116">
-      <c r="A116" s="2" t="n">
+    <row r="116" spans="1:4">
+      <c r="A116" s="2">
         <v>41395</v>
       </c>
-      <c r="B116" t="n">
+      <c r="B116">
         <v>84980000000000</v>
       </c>
-      <c r="C116" t="n">
+      <c r="C116">
         <v>0.0008733624454148472</v>
       </c>
-      <c r="D116" t="n">
+      <c r="D116">
         <v>74218340611.35371</v>
       </c>
     </row>
-    <row r="117">
-      <c r="A117" s="2" t="n">
+    <row r="117" spans="1:4">
+      <c r="A117" s="2">
         <v>41426</v>
       </c>
-      <c r="B117" t="n">
+      <c r="B117">
         <v>85218500000000</v>
       </c>
-      <c r="C117" t="n">
+      <c r="C117">
         <v>0.0008619203585588691</v>
       </c>
-      <c r="D117" t="n">
+      <c r="D117">
         <v>73451560075.84898</v>
       </c>
     </row>
-    <row r="118">
-      <c r="A118" s="2" t="n">
+    <row r="118" spans="1:4">
+      <c r="A118" s="2">
         <v>41456</v>
       </c>
-      <c r="B118" t="n">
+      <c r="B118">
         <v>84998400000000</v>
       </c>
-      <c r="C118" t="n">
+      <c r="C118">
         <v>0.0008605851979345956</v>
       </c>
-      <c r="D118" t="n">
+      <c r="D118">
         <v>73148364888.12393</v>
       </c>
     </row>
-    <row r="119">
-      <c r="A119" s="2" t="n">
+    <row r="119" spans="1:4">
+      <c r="A119" s="2">
         <v>41487</v>
       </c>
-      <c r="B119" t="n">
+      <c r="B119">
         <v>83919500000000</v>
       </c>
-      <c r="C119" t="n">
+      <c r="C119">
         <v>0.0008598452278589854</v>
       </c>
-      <c r="D119" t="n">
+      <c r="D119">
         <v>72157781599.31212</v>
       </c>
     </row>
-    <row r="120">
-      <c r="A120" s="2" t="n">
+    <row r="120" spans="1:4">
+      <c r="A120" s="2">
         <v>41518</v>
       </c>
-      <c r="B120" t="n">
+      <c r="B120">
         <v>85886100000000</v>
       </c>
-      <c r="C120" t="n">
+      <c r="C120">
         <v>0.000859180341953776</v>
       </c>
-      <c r="D120" t="n">
+      <c r="D120">
         <v>73791648767.0762</v>
       </c>
     </row>
-    <row r="121">
-      <c r="A121" s="2" t="n">
+    <row r="121" spans="1:4">
+      <c r="A121" s="2">
         <v>41548</v>
       </c>
-      <c r="B121" t="n">
+      <c r="B121">
         <v>86592400000000</v>
       </c>
-      <c r="C121" t="n">
+      <c r="C121">
         <v>0.0008590696275933165</v>
       </c>
-      <c r="D121" t="n">
+      <c r="D121">
         <v>74388900820.4115</v>
       </c>
     </row>
-    <row r="122">
-      <c r="A122" s="2" t="n">
+    <row r="122" spans="1:4">
+      <c r="A122" s="2">
         <v>41579</v>
       </c>
-      <c r="B122" t="n">
+      <c r="B122">
         <v>86959500000000</v>
       </c>
-      <c r="C122" t="n">
+      <c r="C122">
         <v>0.0008614748449345279</v>
       </c>
-      <c r="D122" t="n">
+      <c r="D122">
         <v>74913421778.08408</v>
       </c>
     </row>
-    <row r="123">
-      <c r="A123" s="2" t="n">
+    <row r="123" spans="1:4">
+      <c r="A123" s="2">
         <v>41609</v>
       </c>
-      <c r="B123" t="n">
+      <c r="B123">
         <v>89512100000000</v>
       </c>
-      <c r="C123" t="n">
+      <c r="C123">
         <v>0.0008592541673827118</v>
       </c>
-      <c r="D123" t="n">
+      <c r="D123">
         <v>76913644956.17804</v>
       </c>
     </row>
-    <row r="124">
-      <c r="A124" s="2" t="n">
+    <row r="124" spans="1:4">
+      <c r="A124" s="2">
         <v>41640</v>
       </c>
-      <c r="B124" t="n">
+      <c r="B124">
         <v>90436700000000</v>
       </c>
-      <c r="C124" t="n">
+      <c r="C124">
         <v>0.0008598452278589854</v>
       </c>
-      <c r="D124" t="n">
+      <c r="D124">
         <v>77761564918.31471</v>
       </c>
     </row>
-    <row r="125">
-      <c r="A125" s="2" t="n">
+    <row r="125" spans="1:4">
+      <c r="A125" s="2">
         <v>41671</v>
       </c>
-      <c r="B125" t="n">
+      <c r="B125">
         <v>88921900000000</v>
       </c>
-      <c r="C125" t="n">
+      <c r="C125">
         <v>0.0008598452278589854</v>
       </c>
-      <c r="D125" t="n">
+      <c r="D125">
         <v>76459071367.15392</v>
       </c>
     </row>
-    <row r="126">
-      <c r="A126" s="2" t="n">
+    <row r="126" spans="1:4">
+      <c r="A126" s="2">
         <v>41699</v>
       </c>
-      <c r="B126" t="n">
+      <c r="B126">
         <v>89146400000000</v>
       </c>
-      <c r="C126" t="n">
+      <c r="C126">
         <v>0.0008594757198109154</v>
       </c>
-      <c r="D126" t="n">
+      <c r="D126">
         <v>76619166308.55179</v>
       </c>
     </row>
-    <row r="127">
-      <c r="A127" s="2" t="n">
+    <row r="127" spans="1:4">
+      <c r="A127" s="2">
         <v>41730</v>
       </c>
-      <c r="B127" t="n">
+      <c r="B127">
         <v>90306400000000</v>
       </c>
-      <c r="C127" t="n">
+      <c r="C127">
         <v>0.0008605851979345956</v>
       </c>
-      <c r="D127" t="n">
+      <c r="D127">
         <v>77716351118.76076</v>
       </c>
     </row>
-    <row r="128">
-      <c r="A128" s="2" t="n">
+    <row r="128" spans="1:4">
+      <c r="A128" s="2">
         <v>41760</v>
       </c>
-      <c r="B128" t="n">
+      <c r="B128">
         <v>88797200000000</v>
       </c>
-      <c r="C128" t="n">
+      <c r="C128">
         <v>0.0008602150537634409</v>
       </c>
-      <c r="D128" t="n">
+      <c r="D128">
         <v>76384688172.04301</v>
       </c>
     </row>
-    <row r="129">
-      <c r="A129" s="2" t="n">
+    <row r="129" spans="1:4">
+      <c r="A129" s="2">
         <v>41791</v>
       </c>
-      <c r="B129" t="n">
+      <c r="B129">
         <v>88852200000000</v>
       </c>
-      <c r="C129" t="n">
+      <c r="C129">
         <v>0.0008600670852326481</v>
       </c>
-      <c r="D129" t="n">
+      <c r="D129">
         <v>76418852670.5083</v>
       </c>
     </row>
-    <row r="130">
-      <c r="A130" s="2" t="n">
+    <row r="130" spans="1:4">
+      <c r="A130" s="2">
         <v>41821</v>
       </c>
-      <c r="B130" t="n">
+      <c r="B130">
         <v>88970400000000</v>
       </c>
-      <c r="C130" t="n">
+      <c r="C130">
         <v>0.000859106529209622</v>
       </c>
-      <c r="D130" t="n">
+      <c r="D130">
         <v>76435051546.39175</v>
       </c>
     </row>
-    <row r="131">
-      <c r="A131" s="2" t="n">
+    <row r="131" spans="1:4">
+      <c r="A131" s="2">
         <v>41852</v>
       </c>
-      <c r="B131" t="n">
+      <c r="B131">
         <v>88497600000000</v>
       </c>
-      <c r="C131" t="n">
+      <c r="C131">
         <v>0.0008613264427217916</v>
       </c>
-      <c r="D131" t="n">
+      <c r="D131">
         <v>76225322997.41602</v>
       </c>
     </row>
-    <row r="132">
-      <c r="A132" s="2" t="n">
+    <row r="132" spans="1:4">
+      <c r="A132" s="2">
         <v>41883</v>
       </c>
-      <c r="B132" t="n">
+      <c r="B132">
         <v>89683800000000</v>
       </c>
-      <c r="C132" t="n">
+      <c r="C132">
         <v>0.0008621432882145012</v>
       </c>
-      <c r="D132" t="n">
+      <c r="D132">
         <v>77320286231.57169</v>
       </c>
     </row>
-    <row r="133">
-      <c r="A133" s="2" t="n">
+    <row r="133" spans="1:4">
+      <c r="A133" s="2">
         <v>41913</v>
       </c>
-      <c r="B133" t="n">
+      <c r="B133">
         <v>90633300000000</v>
       </c>
-      <c r="C133" t="n">
+      <c r="C133">
         <v>0.0008605851979345956</v>
       </c>
-      <c r="D133" t="n">
+      <c r="D133">
         <v>77997676419.96558</v>
       </c>
     </row>
-    <row r="134">
-      <c r="A134" s="2" t="n">
+    <row r="134" spans="1:4">
+      <c r="A134" s="2">
         <v>41944</v>
       </c>
-      <c r="B134" t="n">
+      <c r="B134">
         <v>89370900000000</v>
       </c>
-      <c r="C134" t="n">
+      <c r="C134">
         <v>0.0008620689655172414</v>
       </c>
-      <c r="D134" t="n">
+      <c r="D134">
         <v>77043879310.34483</v>
       </c>
     </row>
-    <row r="135">
-      <c r="A135" s="2" t="n">
+    <row r="135" spans="1:4">
+      <c r="A135" s="2">
         <v>41974</v>
       </c>
-      <c r="B135" t="n">
+      <c r="B135">
         <v>92988900000000</v>
       </c>
-      <c r="C135" t="n">
+      <c r="C135">
         <v>0.0008756567425569177</v>
       </c>
-      <c r="D135" t="n">
+      <c r="D135">
         <v>81426357267.95096</v>
       </c>
     </row>
-    <row r="136">
-      <c r="A136" s="2" t="n">
+    <row r="136" spans="1:4">
+      <c r="A136" s="2">
         <v>42005</v>
       </c>
-      <c r="B136" t="n">
+      <c r="B136">
         <v>88444200000000</v>
       </c>
-      <c r="C136" t="n">
+      <c r="C136">
         <v>0.000859106529209622</v>
       </c>
-      <c r="D136" t="n">
+      <c r="D136">
         <v>75982989690.72165</v>
       </c>
     </row>
-    <row r="137">
-      <c r="A137" s="2" t="n">
+    <row r="137" spans="1:4">
+      <c r="A137" s="2">
         <v>42036</v>
       </c>
-      <c r="B137" t="n">
+      <c r="B137">
         <v>88621900000000</v>
       </c>
-      <c r="C137" t="n">
+      <c r="C137">
         <v>0.0008583690987124463</v>
       </c>
-      <c r="D137" t="n">
+      <c r="D137">
         <v>76070300429.18454</v>
       </c>
     </row>
-    <row r="138">
-      <c r="A138" s="2" t="n">
+    <row r="138" spans="1:4">
+      <c r="A138" s="2">
         <v>42064</v>
       </c>
-      <c r="B138" t="n">
+      <c r="B138">
         <v>91248100000000</v>
       </c>
-      <c r="C138" t="n">
+      <c r="C138">
         <v>0.000859106529209622</v>
       </c>
-      <c r="D138" t="n">
+      <c r="D138">
         <v>78391838487.9725</v>
       </c>
     </row>
-    <row r="139">
-      <c r="A139" s="2" t="n">
+    <row r="139" spans="1:4">
+      <c r="A139" s="2">
         <v>42095</v>
       </c>
-      <c r="B139" t="n">
+      <c r="B139">
         <v>91762000000000</v>
       </c>
-      <c r="C139" t="n">
+      <c r="C139">
         <v>0.000859106529209622</v>
       </c>
-      <c r="D139" t="n">
+      <c r="D139">
         <v>78833333333.33333</v>
       </c>
     </row>
-    <row r="140">
-      <c r="A140" s="2" t="n">
+    <row r="140" spans="1:4">
+      <c r="A140" s="2">
         <v>42125</v>
       </c>
-      <c r="B140" t="n">
+      <c r="B140">
         <v>92930000000000</v>
       </c>
-      <c r="C140" t="n">
+      <c r="C140">
         <v>0.0008583690987124463</v>
       </c>
-      <c r="D140" t="n">
+      <c r="D140">
         <v>79768240343.34764</v>
       </c>
     </row>
-    <row r="141">
-      <c r="A141" s="2" t="n">
+    <row r="141" spans="1:4">
+      <c r="A141" s="2">
         <v>42156</v>
       </c>
-      <c r="B141" t="n">
+      <c r="B141">
         <v>91422000000000</v>
       </c>
-      <c r="C141" t="n">
+      <c r="C141">
         <v>0.0008605851979345956</v>
       </c>
-      <c r="D141" t="n">
+      <c r="D141">
         <v>78676419965.5766</v>
       </c>
     </row>
-    <row r="142">
-      <c r="A142" s="2" t="n">
+    <row r="142" spans="1:4">
+      <c r="A142" s="2">
         <v>42186</v>
       </c>
-      <c r="B142" t="n">
+      <c r="B142">
         <v>89513400000000</v>
       </c>
-      <c r="C142" t="n">
+      <c r="C142">
         <v>0.0008650519031141869</v>
       </c>
-      <c r="D142" t="n">
+      <c r="D142">
         <v>77433737024.22145</v>
       </c>
     </row>
-    <row r="143">
-      <c r="A143" s="2" t="n">
+    <row r="143" spans="1:4">
+      <c r="A143" s="2">
         <v>42217</v>
       </c>
-      <c r="B143" t="n">
+      <c r="B143">
         <v>87471100000000</v>
       </c>
-      <c r="C143" t="n">
+      <c r="C143">
         <v>0.0008741258741258741</v>
       </c>
-      <c r="D143" t="n">
+      <c r="D143">
         <v>76460751748.25175</v>
       </c>
     </row>
-    <row r="144">
-      <c r="A144" s="2" t="n">
+    <row r="144" spans="1:4">
+      <c r="A144" s="2">
         <v>42248</v>
       </c>
-      <c r="B144" t="n">
+      <c r="B144">
         <v>87179100000000</v>
       </c>
-      <c r="C144" t="n">
+      <c r="C144">
         <v>0.0008841732979664014</v>
       </c>
-      <c r="D144" t="n">
+      <c r="D144">
         <v>77081432360.74271</v>
       </c>
     </row>
-    <row r="145">
-      <c r="A145" s="2" t="n">
+    <row r="145" spans="1:4">
+      <c r="A145" s="2">
         <v>42278</v>
       </c>
-      <c r="B145" t="n">
+      <c r="B145">
         <v>86752700000000</v>
       </c>
-      <c r="C145" t="n">
+      <c r="C145">
         <v>0.00089126559714795</v>
       </c>
-      <c r="D145" t="n">
+      <c r="D145">
         <v>77319696969.69696</v>
       </c>
     </row>
-    <row r="146">
-      <c r="A146" s="2" t="n">
+    <row r="146" spans="1:4">
+      <c r="A146" s="2">
         <v>42309</v>
       </c>
-      <c r="B146" t="n">
+      <c r="B146">
         <v>85292700000000</v>
       </c>
-      <c r="C146" t="n">
+      <c r="C146">
         <v>0.0009025270758122744</v>
       </c>
-      <c r="D146" t="n">
+      <c r="D146">
         <v>76978971119.13358</v>
       </c>
     </row>
-    <row r="147">
-      <c r="A147" s="2" t="n">
+    <row r="147" spans="1:4">
+      <c r="A147" s="2">
         <v>42339</v>
       </c>
-      <c r="B147" t="n">
+      <c r="B147">
         <v>84527300000000</v>
       </c>
-      <c r="C147" t="n">
+      <c r="C147">
         <v>0.0009132420091324201</v>
       </c>
-      <c r="D147" t="n">
+      <c r="D147">
         <v>77193881278.5388</v>
       </c>
     </row>
-    <row r="148">
-      <c r="A148" s="2" t="n">
+    <row r="148" spans="1:4">
+      <c r="A148" s="2">
         <v>42370</v>
       </c>
-      <c r="B148" t="n">
+      <c r="B148">
         <v>84418200000000</v>
       </c>
-      <c r="C148" t="n">
+      <c r="C148">
         <v>0.000851063829787234</v>
       </c>
-      <c r="D148" t="n">
+      <c r="D148">
         <v>71845276595.74467</v>
       </c>
     </row>
-    <row r="149">
-      <c r="A149" s="2" t="n">
+    <row r="149" spans="1:4">
+      <c r="A149" s="2">
         <v>42401</v>
       </c>
-      <c r="B149" t="n">
+      <c r="B149">
         <v>86573300000000</v>
       </c>
-      <c r="C149" t="n">
+      <c r="C149">
         <v>0.0008503401360544217</v>
       </c>
-      <c r="D149" t="n">
+      <c r="D149">
         <v>73616751700.68027</v>
       </c>
     </row>
-    <row r="150">
-      <c r="A150" s="2" t="n">
+    <row r="150" spans="1:4">
+      <c r="A150" s="2">
         <v>42430</v>
       </c>
-      <c r="B150" t="n">
+      <c r="B150">
         <v>87960800000000</v>
       </c>
-      <c r="C150" t="n">
+      <c r="C150">
         <v>0.0008547008547008547</v>
       </c>
-      <c r="D150" t="n">
+      <c r="D150">
         <v>75180170940.17094</v>
       </c>
     </row>
-    <row r="151">
-      <c r="A151" s="2" t="n">
+    <row r="151" spans="1:4">
+      <c r="A151" s="2">
         <v>42461</v>
       </c>
-      <c r="B151" t="n">
+      <c r="B151">
         <v>89080000000000</v>
       </c>
-      <c r="C151" t="n">
+      <c r="C151">
         <v>0.000847457627118644</v>
       </c>
-      <c r="D151" t="n">
+      <c r="D151">
         <v>75491525423.72881</v>
       </c>
     </row>
-    <row r="152">
-      <c r="A152" s="2" t="n">
+    <row r="152" spans="1:4">
+      <c r="A152" s="2">
         <v>42491</v>
       </c>
-      <c r="B152" t="n">
+      <c r="B152">
         <v>89342300000000</v>
       </c>
-      <c r="C152" t="n">
+      <c r="C152">
         <v>0.0008551393877201983</v>
       </c>
-      <c r="D152" t="n">
+      <c r="D152">
         <v>76400119719.51427</v>
       </c>
     </row>
-    <row r="153">
-      <c r="A153" s="2" t="n">
+    <row r="153" spans="1:4">
+      <c r="A153" s="2">
         <v>42522</v>
       </c>
-      <c r="B153" t="n">
+      <c r="B153">
         <v>88901100000000</v>
       </c>
-      <c r="C153" t="n">
+      <c r="C153">
         <v>0.0008567511994516792</v>
       </c>
-      <c r="D153" t="n">
+      <c r="D153">
         <v>76166124057.57368</v>
       </c>
     </row>
-    <row r="154">
-      <c r="A154" s="2" t="n">
+    <row r="154" spans="1:4">
+      <c r="A154" s="2">
         <v>42552</v>
       </c>
-      <c r="B154" t="n">
+      <c r="B154">
         <v>89925300000000</v>
       </c>
-      <c r="C154" t="n">
+      <c r="C154">
         <v>0.0008561643835616438</v>
       </c>
-      <c r="D154" t="n">
+      <c r="D154">
         <v>76990839041.09589</v>
       </c>
     </row>
-    <row r="155">
-      <c r="A155" s="2" t="n">
+    <row r="155" spans="1:4">
+      <c r="A155" s="2">
         <v>42583</v>
       </c>
-      <c r="B155" t="n">
+      <c r="B155">
         <v>90540600000000</v>
       </c>
-      <c r="C155" t="n">
+      <c r="C155">
         <v>0.0008600670852326481</v>
       </c>
-      <c r="D155" t="n">
+      <c r="D155">
         <v>77870989937.2151</v>
       </c>
     </row>
-    <row r="156">
-      <c r="A156" s="2" t="n">
+    <row r="156" spans="1:4">
+      <c r="A156" s="2">
         <v>42614</v>
       </c>
-      <c r="B156" t="n">
+      <c r="B156">
         <v>91225700000000</v>
       </c>
-      <c r="C156" t="n">
+      <c r="C156">
         <v>0.0008600670852326481</v>
       </c>
-      <c r="D156" t="n">
+      <c r="D156">
         <v>78460221897.30798</v>
       </c>
     </row>
-    <row r="157">
-      <c r="A157" s="2" t="n">
+    <row r="157" spans="1:4">
+      <c r="A157" s="2">
         <v>42644</v>
       </c>
-      <c r="B157" t="n">
+      <c r="B157">
         <v>90685600000000</v>
       </c>
-      <c r="C157" t="n">
+      <c r="C157">
         <v>0.0008583690987124463</v>
       </c>
-      <c r="D157" t="n">
+      <c r="D157">
         <v>77841716738.19742</v>
       </c>
     </row>
-    <row r="158">
-      <c r="A158" s="2" t="n">
+    <row r="158" spans="1:4">
+      <c r="A158" s="2">
         <v>42675</v>
       </c>
-      <c r="B158" t="n">
+      <c r="B158">
         <v>90106300000000</v>
       </c>
-      <c r="C158" t="n">
+      <c r="C158">
         <v>0.0008617718028266114</v>
       </c>
-      <c r="D158" t="n">
+      <c r="D158">
         <v>77651068597.03549</v>
       </c>
     </row>
-    <row r="159">
-      <c r="A159" s="2" t="n">
+    <row r="159" spans="1:4">
+      <c r="A159" s="2">
         <v>42705</v>
       </c>
-      <c r="B159" t="n">
+      <c r="B159">
         <v>90466400000000</v>
       </c>
-      <c r="C159" t="n">
+      <c r="C159">
         <v>0.000846740050804403</v>
       </c>
-      <c r="D159" t="n">
+      <c r="D159">
         <v>76601524132.09145</v>
       </c>
     </row>
-    <row r="160">
-      <c r="A160" s="2" t="n">
+    <row r="160" spans="1:4">
+      <c r="A160" s="2">
         <v>42736</v>
       </c>
-      <c r="B160" t="n">
+      <c r="B160">
         <v>90454100000000</v>
       </c>
-      <c r="C160" t="n">
+      <c r="C160">
         <v>0.000846740050804403</v>
       </c>
-      <c r="D160" t="n">
+      <c r="D160">
         <v>76591109229.46655</v>
       </c>
     </row>
-    <row r="161">
-      <c r="A161" s="2" t="n">
+    <row r="161" spans="1:4">
+      <c r="A161" s="2">
         <v>42767</v>
       </c>
-      <c r="B161" t="n">
+      <c r="B161">
         <v>90359100000000</v>
       </c>
-      <c r="C161" t="n">
+      <c r="C161">
         <v>0.000846740050804403</v>
       </c>
-      <c r="D161" t="n">
+      <c r="D161">
         <v>76510668924.64014</v>
       </c>
     </row>
-    <row r="162">
-      <c r="A162" s="2" t="n">
+    <row r="162" spans="1:4">
+      <c r="A162" s="2">
         <v>42795</v>
       </c>
-      <c r="B162" t="n">
+      <c r="B162">
         <v>90180100000000</v>
       </c>
-      <c r="C162" t="n">
+      <c r="C162">
         <v>0.000846740050804403</v>
       </c>
-      <c r="D162" t="n">
+      <c r="D162">
         <v>76359102455.54614</v>
       </c>
     </row>
-    <row r="163">
-      <c r="A163" s="2" t="n">
+    <row r="163" spans="1:4">
+      <c r="A163" s="2">
         <v>42826</v>
       </c>
-      <c r="B163" t="n">
+      <c r="B163">
         <v>88855300000000</v>
       </c>
-      <c r="C163" t="n">
+      <c r="C163">
         <v>0.000846740050804403</v>
       </c>
-      <c r="D163" t="n">
+      <c r="D163">
         <v>75237341236.24048</v>
       </c>
     </row>
-    <row r="164">
-      <c r="A164" s="2" t="n">
+    <row r="164" spans="1:4">
+      <c r="A164" s="2">
         <v>42856</v>
       </c>
-      <c r="B164" t="n">
+      <c r="B164">
         <v>89550600000000</v>
       </c>
-      <c r="C164" t="n">
+      <c r="C164">
         <v>0.000846740050804403</v>
       </c>
-      <c r="D164" t="n">
+      <c r="D164">
         <v>75826079593.56477</v>
       </c>
     </row>
-    <row r="165">
-      <c r="A165" s="2" t="n">
+    <row r="165" spans="1:4">
+      <c r="A165" s="2">
         <v>42887</v>
       </c>
-      <c r="B165" t="n">
+      <c r="B165">
         <v>90045300000000</v>
       </c>
-      <c r="C165" t="n">
+      <c r="C165">
         <v>0.000846740050804403</v>
       </c>
-      <c r="D165" t="n">
+      <c r="D165">
         <v>76244961896.69771</v>
       </c>
     </row>
-    <row r="166">
-      <c r="A166" s="2" t="n">
+    <row r="166" spans="1:4">
+      <c r="A166" s="2">
         <v>42917</v>
       </c>
-      <c r="B166" t="n">
+      <c r="B166">
         <v>91205200000000</v>
       </c>
-      <c r="C166" t="n">
+      <c r="C166">
         <v>0.000856898029134533</v>
       </c>
-      <c r="D166" t="n">
+      <c r="D166">
         <v>78153556126.82091</v>
       </c>
     </row>
-    <row r="167">
-      <c r="A167" s="2" t="n">
+    <row r="167" spans="1:4">
+      <c r="A167" s="2">
         <v>42948</v>
       </c>
-      <c r="B167" t="n">
+      <c r="B167">
         <v>90812000000000</v>
       </c>
-      <c r="C167" t="n">
+      <c r="C167">
         <v>0.0008576329331046312</v>
       </c>
-      <c r="D167" t="n">
+      <c r="D167">
         <v>77883361921.09776</v>
       </c>
     </row>
-    <row r="168">
-      <c r="A168" s="2" t="n">
+    <row r="168" spans="1:4">
+      <c r="A168" s="2">
         <v>42979</v>
       </c>
-      <c r="B168" t="n">
+      <c r="B168">
         <v>89870600000000</v>
       </c>
-      <c r="C168" t="n">
+      <c r="C168">
         <v>0.0008576329331046312</v>
       </c>
-      <c r="D168" t="n">
+      <c r="D168">
         <v>77075986277.87306</v>
       </c>
     </row>
-    <row r="169">
-      <c r="A169" s="2" t="n">
+    <row r="169" spans="1:4">
+      <c r="A169" s="2">
         <v>43009</v>
       </c>
-      <c r="B169" t="n">
+      <c r="B169">
         <v>89904900000000</v>
       </c>
-      <c r="C169" t="n">
+      <c r="C169">
         <v>0.0008460236886632825</v>
       </c>
-      <c r="D169" t="n">
+      <c r="D169">
         <v>76061675126.90355</v>
       </c>
     </row>
-    <row r="170">
-      <c r="A170" s="2" t="n">
+    <row r="170" spans="1:4">
+      <c r="A170" s="2">
         <v>43040</v>
       </c>
-      <c r="B170" t="n">
+      <c r="B170">
         <v>91129900000000</v>
       </c>
-      <c r="C170" t="n">
+      <c r="C170">
         <v>0.0008454514710855598</v>
       </c>
-      <c r="D170" t="n">
+      <c r="D170">
         <v>77045908014.87996</v>
       </c>
     </row>
-    <row r="171">
-      <c r="A171" s="2" t="n">
+    <row r="171" spans="1:4">
+      <c r="A171" s="2">
         <v>43070</v>
       </c>
-      <c r="B171" t="n">
+      <c r="B171">
         <v>92857000000000</v>
       </c>
-      <c r="C171" t="n">
+      <c r="C171">
         <v>0.0008445945945945946</v>
       </c>
-      <c r="D171" t="n">
+      <c r="D171">
         <v>78426520270.27028</v>
       </c>
     </row>
-    <row r="172">
-      <c r="A172" s="2" t="n">
+    <row r="172" spans="1:4">
+      <c r="A172" s="2">
         <v>43101</v>
       </c>
-      <c r="B172" t="n">
+      <c r="B172">
         <v>91625200000000</v>
       </c>
-      <c r="C172" t="n">
+      <c r="C172">
         <v>0.0008445945945945946</v>
       </c>
-      <c r="D172" t="n">
+      <c r="D172">
         <v>77386148648.64865</v>
       </c>
     </row>
-    <row r="173">
-      <c r="A173" s="2" t="n">
+    <row r="173" spans="1:4">
+      <c r="A173" s="2">
         <v>43132</v>
       </c>
-      <c r="B173" t="n">
+      <c r="B173">
         <v>90831200000000</v>
       </c>
-      <c r="C173" t="n">
+      <c r="C173">
         <v>0.0008445945945945946</v>
       </c>
-      <c r="D173" t="n">
+      <c r="D173">
         <v>76715540540.54054</v>
       </c>
     </row>
-    <row r="174">
-      <c r="A174" s="2" t="n">
+    <row r="174" spans="1:4">
+      <c r="A174" s="2">
         <v>43160</v>
       </c>
-      <c r="B174" t="n">
+      <c r="B174">
         <v>89517300000000</v>
       </c>
-      <c r="C174" t="n">
+      <c r="C174">
         <v>0.0008445945945945946</v>
       </c>
-      <c r="D174" t="n">
+      <c r="D174">
         <v>75605827702.70271</v>
       </c>
     </row>
-    <row r="175">
-      <c r="A175" s="2" t="n">
+    <row r="175" spans="1:4">
+      <c r="A175" s="2">
         <v>43191</v>
       </c>
-      <c r="B175" t="n">
+      <c r="B175">
         <v>89802800000000</v>
       </c>
-      <c r="C175" t="n">
+      <c r="C175">
         <v>0.0008445945945945946</v>
       </c>
-      <c r="D175" t="n">
+      <c r="D175">
         <v>75846959459.45946</v>
       </c>
     </row>
-    <row r="176">
-      <c r="A176" s="2" t="n">
+    <row r="176" spans="1:4">
+      <c r="A176" s="2">
         <v>43221</v>
       </c>
-      <c r="B176" t="n">
+      <c r="B176">
         <v>88948000000000</v>
       </c>
-      <c r="C176" t="n">
+      <c r="C176">
         <v>0.0008445945945945946</v>
       </c>
-      <c r="D176" t="n">
+      <c r="D176">
         <v>75125000000</v>
       </c>
     </row>
-    <row r="177">
-      <c r="A177" s="2" t="n">
+    <row r="177" spans="1:4">
+      <c r="A177" s="2">
         <v>43252</v>
       </c>
-      <c r="B177" t="n">
+      <c r="B177">
         <v>90973300000000</v>
       </c>
-      <c r="C177" t="n">
+      <c r="C177">
         <v>0.0008445945945945946</v>
       </c>
-      <c r="D177" t="n">
+      <c r="D177">
         <v>76835557432.43243</v>
       </c>
     </row>
-    <row r="178">
-      <c r="A178" s="2" t="n">
+    <row r="178" spans="1:4">
+      <c r="A178" s="2">
         <v>43282</v>
       </c>
-      <c r="B178" t="n">
+      <c r="B178">
         <v>90927900000000</v>
       </c>
-      <c r="C178" t="n">
+      <c r="C178">
         <v>0.0008403361344537816</v>
       </c>
-      <c r="D178" t="n">
+      <c r="D178">
         <v>76410000000</v>
       </c>
     </row>
-    <row r="179">
-      <c r="A179" s="2" t="n">
+    <row r="179" spans="1:4">
+      <c r="A179" s="2">
         <v>43313</v>
       </c>
-      <c r="B179" t="n">
+      <c r="B179">
         <v>91487600000000</v>
       </c>
-      <c r="C179" t="n">
+      <c r="C179">
         <v>0.0008403361344537816</v>
       </c>
-      <c r="D179" t="n">
+      <c r="D179">
         <v>76880336134.45378</v>
       </c>
     </row>
-    <row r="180">
-      <c r="A180" s="2" t="n">
+    <row r="180" spans="1:4">
+      <c r="A180" s="2">
         <v>43344</v>
       </c>
-      <c r="B180" t="n">
+      <c r="B180">
         <v>93170000000000</v>
       </c>
-      <c r="C180" t="n">
+      <c r="C180">
         <v>0.0008403361344537816</v>
       </c>
-      <c r="D180" t="n">
+      <c r="D180">
         <v>78294117647.05882</v>
       </c>
     </row>
-    <row r="181">
-      <c r="A181" s="2" t="n">
+    <row r="181" spans="1:4">
+      <c r="A181" s="2">
         <v>43374</v>
       </c>
-      <c r="B181" t="n">
+      <c r="B181">
         <v>92856900000000</v>
       </c>
-      <c r="C181" t="n">
+      <c r="C181">
         <v>0.0008410428931875525</v>
       </c>
-      <c r="D181" t="n">
+      <c r="D181">
         <v>78096635828.42725</v>
       </c>
     </row>
-    <row r="182">
-      <c r="A182" s="2" t="n">
+    <row r="182" spans="1:4">
+      <c r="A182" s="2">
         <v>43405</v>
       </c>
-      <c r="B182" t="n">
+      <c r="B182">
         <v>93702100000000</v>
       </c>
-      <c r="C182" t="n">
+      <c r="C182">
         <v>0.0008403361344537816</v>
       </c>
-      <c r="D182" t="n">
+      <c r="D182">
         <v>78741260504.20169</v>
       </c>
     </row>
-    <row r="183">
-      <c r="A183" s="2" t="n">
+    <row r="183" spans="1:4">
+      <c r="A183" s="2">
         <v>43435</v>
       </c>
-      <c r="B183" t="n">
+      <c r="B183">
         <v>95390700000000</v>
       </c>
-      <c r="C183" t="n">
+      <c r="C183">
         <v>0.0008410428931875525</v>
       </c>
-      <c r="D183" t="n">
+      <c r="D183">
         <v>80227670311.18587</v>
       </c>
     </row>
-    <row r="184">
-      <c r="A184" s="2" t="n">
+    <row r="184" spans="1:4">
+      <c r="A184" s="2">
         <v>43466</v>
       </c>
-      <c r="B184" t="n">
+      <c r="B184">
         <v>94253000000000</v>
       </c>
-      <c r="C184" t="n">
+      <c r="C184">
         <v>0.0008431703204047217</v>
       </c>
-      <c r="D184" t="n">
+      <c r="D184">
         <v>79471332209.10623</v>
       </c>
     </row>
-    <row r="185">
-      <c r="A185" s="2" t="n">
+    <row r="185" spans="1:4">
+      <c r="A185" s="2">
         <v>43497</v>
       </c>
-      <c r="B185" t="n">
+      <c r="B185">
         <v>93722400000000</v>
       </c>
-      <c r="C185" t="n">
+      <c r="C185">
         <v>0.0008403361344537816</v>
       </c>
-      <c r="D185" t="n">
+      <c r="D185">
         <v>78758319327.73109</v>
       </c>
     </row>
-    <row r="186">
-      <c r="A186" s="2" t="n">
+    <row r="186" spans="1:4">
+      <c r="A186" s="2">
         <v>43525</v>
       </c>
-      <c r="B186" t="n">
+      <c r="B186">
         <v>95621700000000</v>
       </c>
-      <c r="C186" t="n">
+      <c r="C186">
         <v>0.0008410428931875525</v>
       </c>
-      <c r="D186" t="n">
+      <c r="D186">
         <v>80421951219.51219</v>
       </c>
     </row>
-    <row r="187">
-      <c r="A187" s="2" t="n">
+    <row r="187" spans="1:4">
+      <c r="A187" s="2">
         <v>43556</v>
       </c>
-      <c r="B187" t="n">
+      <c r="B187">
         <v>97104100000000</v>
       </c>
-      <c r="C187" t="n">
+      <c r="C187">
         <v>0.0008403361344537816</v>
       </c>
-      <c r="D187" t="n">
+      <c r="D187">
         <v>81600084033.61345</v>
       </c>
     </row>
-    <row r="188">
-      <c r="A188" s="2" t="n">
+    <row r="188" spans="1:4">
+      <c r="A188" s="2">
         <v>43586</v>
       </c>
-      <c r="B188" t="n">
+      <c r="B188">
         <v>96043100000000</v>
       </c>
-      <c r="C188" t="n">
+      <c r="C188">
         <v>0.0008403361344537816</v>
       </c>
-      <c r="D188" t="n">
+      <c r="D188">
         <v>80708487394.95799</v>
       </c>
     </row>
-    <row r="189">
-      <c r="A189" s="2" t="n">
+    <row r="189" spans="1:4">
+      <c r="A189" s="2">
         <v>43617</v>
       </c>
-      <c r="B189" t="n">
+      <c r="B189">
         <v>98466300000000</v>
       </c>
-      <c r="C189" t="n">
+      <c r="C189">
         <v>0.0008403361344537816</v>
       </c>
-      <c r="D189" t="n">
+      <c r="D189">
         <v>82744789915.96638</v>
       </c>
     </row>
-    <row r="190">
-      <c r="A190" s="2" t="n">
+    <row r="190" spans="1:4">
+      <c r="A190" s="2">
         <v>43647</v>
       </c>
-      <c r="B190" t="n">
+      <c r="B190">
         <v>99502000000000</v>
       </c>
-      <c r="C190" t="n">
+      <c r="C190">
         <v>0.0008403361344537816</v>
       </c>
-      <c r="D190" t="n">
+      <c r="D190">
         <v>83615126050.42017</v>
       </c>
     </row>
-    <row r="191">
-      <c r="A191" s="2" t="n">
+    <row r="191" spans="1:4">
+      <c r="A191" s="2">
         <v>43678</v>
       </c>
-      <c r="B191" t="n">
+      <c r="B191">
         <v>100943700000000</v>
       </c>
-      <c r="C191" t="n">
+      <c r="C191">
         <v>0.0008410428931875525</v>
       </c>
-      <c r="D191" t="n">
+      <c r="D191">
         <v>84897981497.05635</v>
       </c>
     </row>
-    <row r="192">
-      <c r="A192" s="2" t="n">
+    <row r="192" spans="1:4">
+      <c r="A192" s="2">
         <v>43709</v>
       </c>
-      <c r="B192" t="n">
+      <c r="B192">
         <v>101802900000000</v>
       </c>
-      <c r="C192" t="n">
+      <c r="C192">
         <v>0.0008410428931875525</v>
       </c>
-      <c r="D192" t="n">
+      <c r="D192">
         <v>85620605550.88309</v>
       </c>
     </row>
-    <row r="193">
-      <c r="A193" s="2" t="n">
+    <row r="193" spans="1:4">
+      <c r="A193" s="2">
         <v>43739</v>
       </c>
-      <c r="B193" t="n">
+      <c r="B193">
         <v>102720000000000</v>
       </c>
-      <c r="C193" t="n">
+      <c r="C193">
         <v>0.0008410428931875525</v>
       </c>
-      <c r="D193" t="n">
+      <c r="D193">
         <v>86391925988.2254</v>
       </c>
     </row>
-    <row r="194">
-      <c r="A194" s="2" t="n">
+    <row r="194" spans="1:4">
+      <c r="A194" s="2">
         <v>43770</v>
       </c>
-      <c r="B194" t="n">
+      <c r="B194">
         <v>102822000000000</v>
       </c>
-      <c r="C194" t="n">
+      <c r="C194">
         <v>0.0008410428931875525</v>
       </c>
-      <c r="D194" t="n">
+      <c r="D194">
         <v>86477712363.33052</v>
       </c>
     </row>
-    <row r="195">
-      <c r="A195" s="2" t="n">
+    <row r="195" spans="1:4">
+      <c r="A195" s="2">
         <v>43800</v>
       </c>
-      <c r="B195" t="n">
+      <c r="B195">
         <v>103440000000000</v>
       </c>
-      <c r="C195" t="n">
+      <c r="C195">
         <v>0.0008410428931875525</v>
       </c>
-      <c r="D195" t="n">
+      <c r="D195">
         <v>86997476871.32043</v>
       </c>
     </row>
-    <row r="196">
-      <c r="A196" s="2" t="n">
+    <row r="196" spans="1:4">
+      <c r="A196" s="2">
         <v>43831</v>
       </c>
-      <c r="B196" t="n">
+      <c r="B196">
         <v>102530000000000</v>
       </c>
-      <c r="C196" t="n">
+      <c r="C196">
         <v>0.0008424599831508003</v>
       </c>
-      <c r="D196" t="n">
+      <c r="D196">
         <v>86377422072.45155</v>
       </c>
     </row>
-    <row r="197">
-      <c r="A197" s="2" t="n">
+    <row r="197" spans="1:4">
+      <c r="A197" s="2">
         <v>43862</v>
       </c>
-      <c r="B197" t="n">
+      <c r="B197">
         <v>105677000000000</v>
       </c>
-      <c r="C197" t="n">
+      <c r="C197">
         <v>0.0008410428931875525</v>
       </c>
-      <c r="D197" t="n">
+      <c r="D197">
         <v>88878889823.38098</v>
       </c>
     </row>
-    <row r="198">
-      <c r="A198" s="2" t="n">
+    <row r="198" spans="1:4">
+      <c r="A198" s="2">
         <v>43891</v>
       </c>
-      <c r="B198" t="n">
+      <c r="B198">
         <v>108215000000000</v>
       </c>
-      <c r="C198" t="n">
+      <c r="C198">
         <v>0.0008410428931875525</v>
       </c>
-      <c r="D198" t="n">
+      <c r="D198">
         <v>91013456686.291</v>
       </c>
     </row>
-    <row r="199">
-      <c r="A199" s="2" t="n">
+    <row r="199" spans="1:4">
+      <c r="A199" s="2">
         <v>43922</v>
       </c>
-      <c r="B199" t="n">
+      <c r="B199">
         <v>110696000000000</v>
       </c>
-      <c r="C199" t="n">
+      <c r="C199">
         <v>0.0008431703204047217</v>
       </c>
-      <c r="D199" t="n">
+      <c r="D199">
         <v>93335581787.52107</v>
       </c>
     </row>
-    <row r="200">
-      <c r="A200" s="2" t="n">
+    <row r="200" spans="1:4">
+      <c r="A200" s="2">
         <v>43952</v>
       </c>
-      <c r="B200" t="n">
+      <c r="B200">
         <v>110015000000000</v>
       </c>
-      <c r="C200" t="n">
+      <c r="C200">
         <v>0.0008410428931875525</v>
       </c>
-      <c r="D200" t="n">
+      <c r="D200">
         <v>92527333894.02859</v>
       </c>
     </row>
-    <row r="201">
-      <c r="A201" s="2" t="n">
+    <row r="201" spans="1:4">
+      <c r="A201" s="2">
         <v>43983</v>
       </c>
-      <c r="B201" t="n">
+      <c r="B201">
         <v>110254000000000</v>
       </c>
-      <c r="C201" t="n">
+      <c r="C201">
         <v>0.0008410428931875525</v>
       </c>
-      <c r="D201" t="n">
+      <c r="D201">
         <v>92728343145.50041</v>
       </c>
     </row>
-    <row r="202">
-      <c r="A202" s="2" t="n">
+    <row r="202" spans="1:4">
+      <c r="A202" s="2">
         <v>44013</v>
       </c>
-      <c r="B202" t="n">
+      <c r="B202">
         <v>111107000000000</v>
       </c>
-      <c r="C202" t="n">
+      <c r="C202">
         <v>0.0008410428931875525</v>
       </c>
-      <c r="D202" t="n">
+      <c r="D202">
         <v>93445752733.3894</v>
       </c>
     </row>
-    <row r="203">
-      <c r="A203" s="2" t="n">
+    <row r="203" spans="1:4">
+      <c r="A203" s="2">
         <v>44044</v>
       </c>
-      <c r="B203" t="n">
+      <c r="B203">
         <v>111677000000000</v>
       </c>
-      <c r="C203" t="n">
+      <c r="C203">
         <v>0.0008410428931875525</v>
       </c>
-      <c r="D203" t="n">
+      <c r="D203">
         <v>93925147182.5063</v>
       </c>
     </row>
-    <row r="204">
-      <c r="A204" s="2" t="n">
+    <row r="204" spans="1:4">
+      <c r="A204" s="2">
         <v>44075</v>
       </c>
-      <c r="B204" t="n">
+      <c r="B204">
         <v>112498000000000</v>
       </c>
-      <c r="C204" t="n">
+      <c r="C204">
         <v>0.0008410428931875525</v>
       </c>
-      <c r="D204" t="n">
+      <c r="D204">
         <v>94615643397.81328</v>
       </c>
     </row>
-    <row r="205">
-      <c r="A205" s="2" t="n">
+    <row r="205" spans="1:4">
+      <c r="A205" s="2">
         <v>44105</v>
       </c>
-      <c r="B205" t="n">
+      <c r="B205">
         <v>111829000000000</v>
       </c>
-      <c r="C205" t="n">
+      <c r="C205">
         <v>0.0008438818565400844</v>
       </c>
-      <c r="D205" t="n">
+      <c r="D205">
         <v>94370464135.0211</v>
       </c>
     </row>
-    <row r="206">
-      <c r="A206" s="2" t="n">
+    <row r="206" spans="1:4">
+      <c r="A206" s="2">
         <v>44136</v>
       </c>
-      <c r="B206" t="n">
+      <c r="B206">
         <v>113740000000000</v>
       </c>
-      <c r="C206" t="n">
+      <c r="C206">
         <v>0.0008410428931875525</v>
       </c>
-      <c r="D206" t="n">
+      <c r="D206">
         <v>95660218671.15222</v>
       </c>
     </row>
-    <row r="207">
-      <c r="A207" s="2" t="n">
+    <row r="207" spans="1:4">
+      <c r="A207" s="2">
         <v>44166</v>
       </c>
-      <c r="B207" t="n">
+      <c r="B207">
         <v>119906000000000</v>
       </c>
-      <c r="C207" t="n">
+      <c r="C207">
         <v>0.0006849315068493151</v>
       </c>
-      <c r="D207" t="n">
+      <c r="D207">
         <v>82127397260.27397</v>
       </c>
     </row>
-    <row r="208">
-      <c r="A208" s="2" t="n">
+    <row r="208" spans="1:4">
+      <c r="A208" s="2">
         <v>44197</v>
       </c>
-      <c r="B208" t="n">
+      <c r="B208">
         <v>122037000000000</v>
       </c>
-      <c r="C208" t="n">
+      <c r="C208">
         <v>0.0006849315068493151</v>
       </c>
-      <c r="D208" t="n">
+      <c r="D208">
         <v>83586986301.36986</v>
       </c>
     </row>
-    <row r="209">
-      <c r="A209" s="2" t="n">
+    <row r="209" spans="1:4">
+      <c r="A209" s="2">
         <v>44228</v>
       </c>
-      <c r="B209" t="n">
+      <c r="B209">
         <v>125762000000000</v>
       </c>
-      <c r="C209" t="n">
+      <c r="C209">
         <v>0.0006858710562414266</v>
       </c>
-      <c r="D209" t="n">
+      <c r="D209">
         <v>86256515775.03429</v>
       </c>
     </row>
-    <row r="210">
-      <c r="A210" s="2" t="n">
+    <row r="210" spans="1:4">
+      <c r="A210" s="2">
         <v>44256</v>
       </c>
-      <c r="B210" t="n">
+      <c r="B210">
         <v>128693000000000</v>
       </c>
-      <c r="C210" t="n">
+      <c r="C210">
         <v>0.0006858710562414266</v>
       </c>
-      <c r="D210" t="n">
+      <c r="D210">
         <v>88266803840.87791</v>
       </c>
     </row>
-    <row r="211">
-      <c r="A211" s="2" t="n">
+    <row r="211" spans="1:4">
+      <c r="A211" s="2">
         <v>44287</v>
       </c>
-      <c r="B211" t="n">
+      <c r="B211">
         <v>129860000000000</v>
       </c>
-      <c r="C211" t="n">
+      <c r="C211">
         <v>0.0006858710562414266</v>
       </c>
-      <c r="D211" t="n">
+      <c r="D211">
         <v>89067215363.51166</v>
       </c>
     </row>
-    <row r="212">
-      <c r="A212" s="2" t="n">
+    <row r="212" spans="1:4">
+      <c r="A212" s="2">
         <v>44317</v>
       </c>
-      <c r="B212" t="n">
+      <c r="B212">
         <v>132950000000000</v>
       </c>
-      <c r="C212" t="n">
+      <c r="C212">
         <v>0.0006858710562414266</v>
       </c>
-      <c r="D212" t="n">
+      <c r="D212">
         <v>91186556927.29767</v>
       </c>
     </row>
-    <row r="213">
-      <c r="A213" s="2" t="n">
+    <row r="213" spans="1:4">
+      <c r="A213" s="2">
         <v>44348</v>
       </c>
-      <c r="B213" t="n">
+      <c r="B213">
         <v>133546000000000</v>
       </c>
-      <c r="C213" t="n">
+      <c r="C213">
         <v>0.0006858710562414266</v>
       </c>
-      <c r="D213" t="n">
+      <c r="D213">
         <v>91595336076.81755</v>
       </c>
     </row>
-    <row r="214">
-      <c r="A214" s="2" t="n">
+    <row r="214" spans="1:4">
+      <c r="A214" s="2">
         <v>44378</v>
       </c>
-      <c r="B214" t="n">
+      <c r="B214">
         <v>134911000000000</v>
       </c>
-      <c r="C214" t="n">
+      <c r="C214">
         <v>0.0006858710562414266</v>
       </c>
-      <c r="D214" t="n">
+      <c r="D214">
         <v>92531550068.5871</v>
       </c>
     </row>
-    <row r="215">
-      <c r="A215" s="2" t="n">
+    <row r="215" spans="1:4">
+      <c r="A215" s="2">
         <v>44409</v>
       </c>
-      <c r="B215" t="n">
+      <c r="B215">
         <v>135604000000000</v>
       </c>
-      <c r="C215" t="n">
+      <c r="C215">
         <v>0.0006858710562414266</v>
       </c>
-      <c r="D215" t="n">
+      <c r="D215">
         <v>93006858710.56241</v>
       </c>
     </row>
-    <row r="216">
-      <c r="A216" s="2" t="n">
+    <row r="216" spans="1:4">
+      <c r="A216" s="2">
         <v>44440</v>
       </c>
-      <c r="B216" t="n">
+      <c r="B216">
         <v>135101000000000</v>
       </c>
-      <c r="C216" t="n">
+      <c r="C216">
         <v>0.0006854009595613434</v>
       </c>
-      <c r="D216" t="n">
+      <c r="D216">
         <v>92598355037.69705</v>
       </c>
     </row>
-    <row r="217">
-      <c r="A217" s="2" t="n">
+    <row r="217" spans="1:4">
+      <c r="A217" s="2">
         <v>44470</v>
       </c>
-      <c r="B217" t="n">
+      <c r="B217">
         <v>137856000000000</v>
       </c>
-      <c r="C217" t="n">
+      <c r="C217">
         <v>0.0006858710562414266</v>
       </c>
-      <c r="D217" t="n">
+      <c r="D217">
         <v>94551440329.21809</v>
       </c>
     </row>
-    <row r="218">
-      <c r="A218" s="2" t="n">
+    <row r="218" spans="1:4">
+      <c r="A218" s="2">
         <v>44501</v>
       </c>
-      <c r="B218" t="n">
+      <c r="B218">
         <v>136915000000000</v>
       </c>
-      <c r="C218" t="n">
+      <c r="C218">
         <v>0.0006858710562414266</v>
       </c>
-      <c r="D218" t="n">
+      <c r="D218">
         <v>93906035665.29492</v>
       </c>
     </row>
-    <row r="219">
-      <c r="A219" s="2" t="n">
+    <row r="219" spans="1:4">
+      <c r="A219" s="2">
         <v>44531</v>
       </c>
-      <c r="B219" t="n">
+      <c r="B219">
         <v>139886000000000</v>
       </c>
-      <c r="C219" t="n">
+      <c r="C219">
         <v>0.0006856265255190193</v>
       </c>
-      <c r="D219" t="n">
+      <c r="D219">
         <v>95909552148.75354</v>
       </c>
     </row>
-    <row r="220">
-      <c r="A220" s="2" t="n">
+    <row r="220" spans="1:4">
+      <c r="A220" s="2">
         <v>44562</v>
       </c>
-      <c r="B220" t="n">
+      <c r="B220">
         <v>139567000000000</v>
       </c>
-      <c r="C220" t="n">
+      <c r="C220">
         <v>0.0006856265255190193</v>
       </c>
-      <c r="D220" t="n">
+      <c r="D220">
         <v>95690837287.11296</v>
       </c>
     </row>
-    <row r="221">
-      <c r="A221" s="2" t="n">
+    <row r="221" spans="1:4">
+      <c r="A221" s="2">
         <v>44593</v>
       </c>
-      <c r="B221" t="n">
+      <c r="B221">
         <v>141848000000000</v>
       </c>
-      <c r="C221" t="n">
+      <c r="C221">
         <v>0.0006856359273225917</v>
       </c>
-      <c r="D221" t="n">
+      <c r="D221">
         <v>97256085018.855</v>
       </c>
     </row>
-    <row r="222">
-      <c r="A222" s="2" t="n">
+    <row r="222" spans="1:4">
+      <c r="A222" s="2">
         <v>44621</v>
       </c>
-      <c r="B222" t="n">
+      <c r="B222">
         <v>143176000000000</v>
       </c>
-      <c r="C222" t="n">
+      <c r="C222">
         <v>0.0006856265255190193</v>
       </c>
-      <c r="D222" t="n">
+      <c r="D222">
         <v>98165263417.71111</v>
       </c>
     </row>
-    <row r="223">
-      <c r="A223" s="2" t="n">
+    <row r="223" spans="1:4">
+      <c r="A223" s="2">
         <v>44652</v>
       </c>
-      <c r="B223" t="n">
+      <c r="B223">
         <v>146019000000000</v>
       </c>
-      <c r="C223" t="n">
+      <c r="C223">
         <v>0.0006858710562414266</v>
       </c>
-      <c r="D223" t="n">
+      <c r="D223">
         <v>100150205761.3169</v>
       </c>
     </row>
-    <row r="224">
-      <c r="A224" s="2" t="n">
+    <row r="224" spans="1:4">
+      <c r="A224" s="2">
         <v>44682</v>
       </c>
-      <c r="B224" t="n">
+      <c r="B224">
         <v>146009000000000</v>
       </c>
-      <c r="C224" t="n">
+      <c r="C224">
         <v>0.0006856359273225917</v>
       </c>
-      <c r="D224" t="n">
+      <c r="D224">
         <v>100109016112.4443</v>
       </c>
     </row>
-    <row r="225">
-      <c r="A225" s="2" t="n">
+    <row r="225" spans="1:4">
+      <c r="A225" s="2">
         <v>44713</v>
       </c>
-      <c r="B225" t="n">
+      <c r="B225">
         <v>150010000000000</v>
       </c>
-      <c r="C225" t="n">
+      <c r="C225">
         <v>0.0006856359273225917</v>
       </c>
-      <c r="D225" t="n">
+      <c r="D225">
         <v>102852245457.662</v>
       </c>
     </row>
-    <row r="226">
-      <c r="A226" s="2" t="n">
+    <row r="226" spans="1:4">
+      <c r="A226" s="2">
         <v>44743</v>
       </c>
-      <c r="B226" t="n">
+      <c r="B226">
         <v>151762000000000</v>
       </c>
-      <c r="C226" t="n">
+      <c r="C226">
         <v>0.0006856265255190193</v>
       </c>
-      <c r="D226" t="n">
+      <c r="D226">
         <v>104052052765.8174</v>
       </c>
     </row>
-    <row r="227">
-      <c r="A227" s="2" t="n">
+    <row r="227" spans="1:4">
+      <c r="A227" s="2">
         <v>44774</v>
       </c>
-      <c r="B227" t="n">
+      <c r="B227">
         <v>153983000000000</v>
       </c>
-      <c r="C227" t="n">
+      <c r="C227">
         <v>0.0006856265255190193</v>
       </c>
-      <c r="D227" t="n">
+      <c r="D227">
         <v>105574829278.9951</v>
       </c>
     </row>
-    <row r="228">
-      <c r="A228" s="2" t="n">
+    <row r="228" spans="1:4">
+      <c r="A228" s="2">
         <v>44805</v>
       </c>
-      <c r="B228" t="n">
+      <c r="B228">
         <v>153728000000000</v>
       </c>
-      <c r="C228" t="n">
+      <c r="C228">
         <v>0.0006856218247139243</v>
       </c>
-      <c r="D228" t="n">
+      <c r="D228">
         <v>105399271869.6221</v>
       </c>
     </row>
-    <row r="229">
-      <c r="A229" s="2" t="n">
+    <row r="229" spans="1:4">
+      <c r="A229" s="2">
         <v>44835</v>
       </c>
-      <c r="B229" t="n">
+      <c r="B229">
         <v>157418000000000</v>
       </c>
-      <c r="C229" t="n">
+      <c r="C229">
         <v>0.0006856359273225917</v>
       </c>
-      <c r="D229" t="n">
+      <c r="D229">
         <v>107931436407.2677</v>
       </c>
     </row>
-    <row r="230">
-      <c r="A230" s="2" t="n">
+    <row r="230" spans="1:4">
+      <c r="A230" s="2">
         <v>44866</v>
       </c>
-      <c r="B230" t="n">
+      <c r="B230">
         <v>161714000000000</v>
       </c>
-      <c r="C230" t="n">
+      <c r="C230">
         <v>0.0006856359273225917</v>
       </c>
-      <c r="D230" t="n">
+      <c r="D230">
         <v>110876928351.0456</v>
       </c>
     </row>
-    <row r="231">
-      <c r="A231" s="2" t="n">
+    <row r="231" spans="1:4">
+      <c r="A231" s="2">
         <v>44896</v>
       </c>
-      <c r="B231" t="n">
+      <c r="B231">
         <v>168202000000000</v>
       </c>
-      <c r="C231" t="n">
+      <c r="C231">
         <v>0.0006856171239732884</v>
       </c>
-      <c r="D231" t="n">
+      <c r="D231">
         <v>115322171486.5551</v>
       </c>
     </row>
-    <row r="232">
-      <c r="A232" s="2" t="n">
+    <row r="232" spans="1:4">
+      <c r="A232" s="2">
         <v>44927</v>
       </c>
-      <c r="B232" t="n">
+      <c r="B232">
         <v>171763000000000</v>
       </c>
-      <c r="C232" t="n">
+      <c r="C232">
         <v>0.0006856359273225917</v>
       </c>
-      <c r="D232" t="n">
+      <c r="D232">
         <v>117766883784.7103</v>
       </c>
     </row>
-    <row r="233">
-      <c r="A233" s="2" t="n">
+    <row r="233" spans="1:4">
+      <c r="A233" s="2">
         <v>44958</v>
       </c>
-      <c r="B233" t="n">
+      <c r="B233">
         <v>171365000000000</v>
       </c>
-      <c r="C233" t="n">
+      <c r="C233">
         <v>0.0006856265255190193</v>
       </c>
-      <c r="D233" t="n">
+      <c r="D233">
         <v>117492389545.5667</v>
       </c>
     </row>
-    <row r="234">
-      <c r="A234" s="2" t="n">
+    <row r="234" spans="1:4">
+      <c r="A234" s="2">
         <v>44986</v>
       </c>
-      <c r="B234" t="n">
+      <c r="B234">
         <v>170464000000000</v>
       </c>
-      <c r="C234" t="n">
+      <c r="C234">
         <v>0.0007627765064836003</v>
       </c>
-      <c r="D234" t="n">
+      <c r="D234">
         <v>130025934401.2204</v>
       </c>
     </row>
-    <row r="235">
-      <c r="A235" s="2" t="n">
+    <row r="235" spans="1:4">
+      <c r="A235" s="2">
         <v>45017</v>
       </c>
-      <c r="B235" t="n">
+      <c r="B235">
         <v>173099000000000</v>
       </c>
-      <c r="C235" t="n">
+      <c r="C235">
         <v>0.0007645259938837921</v>
       </c>
-      <c r="D235" t="n">
+      <c r="D235">
         <v>132338685015.2905</v>
       </c>
     </row>
-    <row r="236">
-      <c r="A236" s="2" t="n">
+    <row r="236" spans="1:4">
+      <c r="A236" s="2">
         <v>45047</v>
       </c>
-      <c r="B236" t="n">
+      <c r="B236">
         <v>173504000000000</v>
       </c>
-      <c r="C236" t="n">
+      <c r="C236">
         <v>0.0007639419404125286</v>
       </c>
-      <c r="D236" t="n">
+      <c r="D236">
         <v>132546982429.3354</v>
       </c>
     </row>
-    <row r="237">
-      <c r="A237" s="2" t="n">
+    <row r="237" spans="1:4">
+      <c r="A237" s="2">
         <v>45078</v>
       </c>
-      <c r="B237" t="n">
+      <c r="B237">
         <v>177772000000000</v>
       </c>
-      <c r="C237" t="n">
+      <c r="C237">
         <v>0.0007651109410864575</v>
       </c>
-      <c r="D237" t="n">
+      <c r="D237">
         <v>136015302218.8217</v>
       </c>
     </row>
-    <row r="238">
-      <c r="A238" s="2" t="n">
+    <row r="238" spans="1:4">
+      <c r="A238" s="2">
         <v>45108</v>
       </c>
-      <c r="B238" t="n">
+      <c r="B238">
         <v>176788000000000</v>
       </c>
-      <c r="C238" t="n">
+      <c r="C238">
         <v>0.0007645259938837921</v>
       </c>
-      <c r="D238" t="n">
+      <c r="D238">
         <v>135159021406.7278</v>
       </c>
     </row>
-    <row r="239">
-      <c r="A239" s="2" t="n">
+    <row r="239" spans="1:4">
+      <c r="A239" s="2">
         <v>45139</v>
       </c>
-      <c r="B239" t="n">
+      <c r="B239">
         <v>174322000000000</v>
       </c>
-      <c r="C239" t="n">
+      <c r="C239">
         <v>0.0007641637755803825</v>
       </c>
-      <c r="D239" t="n">
+      <c r="D239">
         <v>133210557686.7234</v>
       </c>
     </row>
-    <row r="240">
-      <c r="A240" s="2" t="n">
+    <row r="240" spans="1:4">
+      <c r="A240" s="2">
         <v>45170</v>
       </c>
-      <c r="B240" t="n">
+      <c r="B240">
         <v>173950000000000</v>
       </c>
-      <c r="C240" t="n">
+      <c r="C240">
         <v>0.0007641637755803825</v>
       </c>
-      <c r="D240" t="n">
+      <c r="D240">
         <v>132926288762.2075</v>
       </c>
     </row>
-    <row r="241">
-      <c r="A241" s="2" t="n">
+    <row r="241" spans="1:4">
+      <c r="A241" s="2">
         <v>45200</v>
       </c>
-      <c r="B241" t="n">
+      <c r="B241">
         <v>176305000000000</v>
       </c>
-      <c r="C241" t="n">
+      <c r="C241">
         <v>0.0007639419404125286</v>
       </c>
-      <c r="D241" t="n">
+      <c r="D241">
         <v>134686783804.4309</v>
       </c>
     </row>
-    <row r="242">
-      <c r="A242" s="2" t="n">
+    <row r="242" spans="1:4">
+      <c r="A242" s="2">
         <v>45231</v>
       </c>
-      <c r="B242" t="n">
-        <v>178918000000000</v>
-      </c>
-      <c r="C242" t="n">
+      <c r="B242">
+        <v>178890000000000</v>
+      </c>
+      <c r="C242">
         <v>0.0007639419404125286</v>
       </c>
-      <c r="D242" t="n">
-        <v>136682964094.7288</v>
+      <c r="D242">
+        <v>136661573720.3972</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>